<commit_message>
Make gen closer to final specification
</commit_message>
<xml_diff>
--- a/Cloud Platforms (PaaS).xlsx
+++ b/Cloud Platforms (PaaS).xlsx
@@ -4237,10 +4237,10 @@
   <dimension ref="A1:AN320"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B84" sqref="B84"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Additions, gen doesn't override diff profiles
</commit_message>
<xml_diff>
--- a/Cloud Platforms (PaaS).xlsx
+++ b/Cloud Platforms (PaaS).xlsx
@@ -1253,7 +1253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="540">
   <si>
     <t>Parent Platform Name</t>
   </si>
@@ -2126,9 +2126,6 @@
   </si>
   <si>
     <t>http://blog.appharbor.com/</t>
-  </si>
-  <si>
-    <t>Monthly Fee</t>
   </si>
   <si>
     <t>AppFog Inc.</t>
@@ -4225,10 +4222,10 @@
   <dimension ref="A1:AO320"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="S16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q68" sqref="Q68"/>
+      <selection pane="bottomRight" activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4289,7 +4286,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="112" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G1" s="224" t="s">
         <v>4</v>
@@ -4323,16 +4320,16 @@
         <v>188</v>
       </c>
       <c r="V1" s="83" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="W1" s="180" t="s">
         <v>78</v>
       </c>
       <c r="X1" s="180" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Y1" s="235" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Z1" s="236"/>
       <c r="AA1" s="73" t="s">
@@ -4357,7 +4354,7 @@
       <c r="AL1" s="222"/>
       <c r="AM1" s="223"/>
       <c r="AN1" s="220" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AO1" s="73" t="s">
         <v>12</v>
@@ -4365,7 +4362,7 @@
     </row>
     <row r="2" spans="1:41" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="232" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C2" s="232"/>
       <c r="D2" s="232"/>
@@ -4390,7 +4387,7 @@
         <v>19</v>
       </c>
       <c r="M2" s="197" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N2" s="200" t="s">
         <v>285</v>
@@ -4409,14 +4406,14 @@
         <v>29</v>
       </c>
       <c r="Z2" s="189" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="AA2" s="74"/>
       <c r="AB2" s="30" t="s">
+        <v>349</v>
+      </c>
+      <c r="AC2" s="6" t="s">
         <v>350</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>351</v>
       </c>
       <c r="AD2" s="6" t="s">
         <v>20</v>
@@ -4428,7 +4425,7 @@
         <v>22</v>
       </c>
       <c r="AG2" s="31" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AH2" s="30" t="s">
         <v>277</v>
@@ -4566,13 +4563,13 @@
     </row>
     <row r="4" spans="1:41" s="63" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="76" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G4" s="201"/>
       <c r="H4" s="11"/>
@@ -4596,11 +4593,11 @@
         <v>215</v>
       </c>
       <c r="T4" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="U4" s="32"/>
       <c r="V4" s="114" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="W4" s="178">
         <v>40878</v>
@@ -4625,7 +4622,7 @@
       <c r="AM4" s="33"/>
       <c r="AN4" s="33"/>
       <c r="AO4" s="76" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -4635,10 +4632,10 @@
       <c r="C5" s="115"/>
       <c r="D5" s="115"/>
       <c r="E5" s="115" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F5" s="116" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G5" s="133"/>
       <c r="H5" s="134"/>
@@ -4652,7 +4649,7 @@
       <c r="N5" s="135"/>
       <c r="O5" s="118"/>
       <c r="P5" s="119" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Q5" s="120" t="s">
         <v>29</v>
@@ -4661,16 +4658,16 @@
         <v>28</v>
       </c>
       <c r="S5" s="122" t="s">
+        <v>384</v>
+      </c>
+      <c r="T5" s="120" t="s">
         <v>385</v>
       </c>
-      <c r="T5" s="120" t="s">
+      <c r="U5" s="117" t="s">
         <v>386</v>
       </c>
-      <c r="U5" s="117" t="s">
+      <c r="V5" s="123" t="s">
         <v>387</v>
-      </c>
-      <c r="V5" s="123" t="s">
-        <v>388</v>
       </c>
       <c r="W5" s="175"/>
       <c r="X5" s="175">
@@ -4685,7 +4682,7 @@
         <v>0</v>
       </c>
       <c r="AA5" s="116" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB5" s="121" t="s">
         <v>25</v>
@@ -4728,7 +4725,7 @@
       <c r="D6" s="124"/>
       <c r="E6" s="124"/>
       <c r="F6" s="125" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G6" s="203" t="s">
         <v>25</v>
@@ -4759,7 +4756,7 @@
         <v>36</v>
       </c>
       <c r="S6" s="130" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="T6" s="129" t="s">
         <v>30</v>
@@ -4783,7 +4780,7 @@
         <v>29</v>
       </c>
       <c r="AA6" s="125" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB6" s="126" t="s">
         <v>25</v>
@@ -4815,7 +4812,7 @@
       </c>
       <c r="AL6" s="124"/>
       <c r="AM6" s="129" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AN6" s="129"/>
       <c r="AO6" s="125"/>
@@ -4828,7 +4825,7 @@
       <c r="D7" s="131"/>
       <c r="E7" s="131"/>
       <c r="F7" s="132" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G7" s="133"/>
       <c r="H7" s="134" t="s">
@@ -4872,14 +4869,14 @@
       </c>
       <c r="Y7" s="192">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Z7" s="194">
         <f t="shared" ca="1" si="3"/>
         <v>31</v>
       </c>
       <c r="AA7" s="132" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB7" s="138" t="s">
         <v>25</v>
@@ -4903,7 +4900,7 @@
       </c>
       <c r="AL7" s="131"/>
       <c r="AM7" s="139" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AN7" s="139"/>
       <c r="AO7" s="116"/>
@@ -4916,7 +4913,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G8" s="206"/>
       <c r="H8" s="206"/>
@@ -4937,10 +4934,10 @@
         <v>155</v>
       </c>
       <c r="S8" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="T8" s="3" t="s">
         <v>390</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>391</v>
       </c>
       <c r="U8" s="3"/>
       <c r="V8" s="7" t="s">
@@ -4951,7 +4948,7 @@
       <c r="Y8" s="192"/>
       <c r="Z8" s="194"/>
       <c r="AA8" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB8" s="3" t="s">
         <v>25</v>
@@ -4977,10 +4974,10 @@
         <v>40</v>
       </c>
       <c r="E9" s="51" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F9" s="158" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G9" s="207" t="s">
         <v>25</v>
@@ -5003,16 +5000,16 @@
         <v>41</v>
       </c>
       <c r="S9" s="51" t="s">
+        <v>354</v>
+      </c>
+      <c r="T9" s="160" t="s">
         <v>355</v>
       </c>
-      <c r="T9" s="160" t="s">
-        <v>356</v>
-      </c>
       <c r="U9" s="159" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="V9" s="51" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="W9" s="183"/>
       <c r="X9" s="183">
@@ -5020,14 +5017,14 @@
       </c>
       <c r="Y9" s="192">
         <f t="shared" ca="1" si="2"/>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Z9" s="194" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="AA9" s="158" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AB9" s="159"/>
       <c r="AG9" s="160"/>
@@ -5047,7 +5044,7 @@
       <c r="AM9" s="160"/>
       <c r="AN9" s="160"/>
       <c r="AO9" s="158" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:41" s="42" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5058,7 +5055,7 @@
         <v>43</v>
       </c>
       <c r="F10" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G10" s="45" t="s">
         <v>25</v>
@@ -5073,7 +5070,7 @@
         <v>44</v>
       </c>
       <c r="M10" s="46" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N10" s="47"/>
       <c r="O10" s="110"/>
@@ -5088,10 +5085,10 @@
         <v>45</v>
       </c>
       <c r="T10" s="54" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="U10" s="53" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="V10" s="65">
         <v>39879</v>
@@ -5109,7 +5106,7 @@
         <v>0</v>
       </c>
       <c r="AA10" s="75" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AB10" s="53"/>
       <c r="AG10" s="54"/>
@@ -5127,7 +5124,7 @@
       <c r="AM10" s="54"/>
       <c r="AN10" s="54"/>
       <c r="AO10" s="75" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11" spans="1:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5138,7 +5135,7 @@
       <c r="D11" s="57"/>
       <c r="E11" s="57"/>
       <c r="F11" s="57" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G11" s="58"/>
       <c r="H11" s="58" t="s">
@@ -5184,10 +5181,10 @@
         <v>47</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F12" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G12" s="45" t="s">
         <v>25</v>
@@ -5216,13 +5213,13 @@
         <v>48</v>
       </c>
       <c r="S12" s="64" t="s">
+        <v>422</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="U12" s="53" t="s">
         <v>423</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="U12" s="53" t="s">
-        <v>424</v>
       </c>
       <c r="V12" s="163">
         <v>40575</v>
@@ -5232,7 +5229,7 @@
       <c r="Y12" s="218"/>
       <c r="Z12" s="219"/>
       <c r="AA12" s="75" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AB12" s="53" t="s">
         <v>25</v>
@@ -5270,7 +5267,7 @@
       <c r="D13" s="115"/>
       <c r="E13" s="115"/>
       <c r="F13" s="116" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G13" s="133"/>
       <c r="H13" s="134"/>
@@ -5297,7 +5294,7 @@
         <v>269</v>
       </c>
       <c r="U13" s="121" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="V13" s="141" t="s">
         <v>270</v>
@@ -5317,7 +5314,7 @@
         <v>72</v>
       </c>
       <c r="AA13" s="116" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB13" s="121"/>
       <c r="AC13" s="115"/>
@@ -5348,7 +5345,7 @@
       </c>
       <c r="E14" s="44"/>
       <c r="F14" s="77" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G14" s="45"/>
       <c r="H14" s="46"/>
@@ -5372,10 +5369,10 @@
         <v>249</v>
       </c>
       <c r="T14" s="54" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="U14" s="53" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="V14" s="65">
         <v>40205</v>
@@ -5393,7 +5390,7 @@
         <v>0</v>
       </c>
       <c r="AA14" s="77" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AB14" s="48"/>
       <c r="AC14" s="44"/>
@@ -5421,10 +5418,10 @@
       <c r="C15" s="115"/>
       <c r="D15" s="115"/>
       <c r="E15" s="115" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F15" s="116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G15" s="133" t="s">
         <v>31</v>
@@ -5441,11 +5438,11 @@
         <v>31</v>
       </c>
       <c r="M15" s="134" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N15" s="135"/>
       <c r="O15" s="142" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P15" s="119"/>
       <c r="Q15" s="120" t="s">
@@ -5461,7 +5458,7 @@
         <v>262</v>
       </c>
       <c r="U15" s="121" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="V15" s="141" t="s">
         <v>275</v>
@@ -5479,7 +5476,7 @@
         <v>0</v>
       </c>
       <c r="AA15" s="116" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB15" s="121"/>
       <c r="AC15" s="115"/>
@@ -5514,7 +5511,7 @@
       <c r="D16" s="115"/>
       <c r="E16" s="115"/>
       <c r="F16" s="116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G16" s="133" t="s">
         <v>25</v>
@@ -5551,7 +5548,7 @@
         <v>217</v>
       </c>
       <c r="U16" s="121" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="V16" s="141" t="s">
         <v>206</v>
@@ -5571,7 +5568,7 @@
         <v>36</v>
       </c>
       <c r="AA16" s="116" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB16" s="121"/>
       <c r="AC16" s="115"/>
@@ -5603,10 +5600,10 @@
       <c r="C17" s="131"/>
       <c r="D17" s="131"/>
       <c r="E17" s="131" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F17" s="132" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G17" s="133" t="s">
         <v>25</v>
@@ -5621,7 +5618,7 @@
         <v>25</v>
       </c>
       <c r="M17" s="134" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N17" s="135" t="s">
         <v>25</v>
@@ -5637,16 +5634,16 @@
         <v>52</v>
       </c>
       <c r="S17" s="122" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="T17" s="139" t="s">
         <v>265</v>
       </c>
       <c r="U17" s="138" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="V17" s="141" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="W17" s="175"/>
       <c r="X17" s="175"/>
@@ -5687,10 +5684,10 @@
       </c>
       <c r="D18" s="124"/>
       <c r="E18" s="124" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F18" s="125" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G18" s="203"/>
       <c r="H18" s="204"/>
@@ -5721,7 +5718,7 @@
         <v>183</v>
       </c>
       <c r="U18" s="121" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="V18" s="124" t="s">
         <v>190</v>
@@ -5755,7 +5752,7 @@
       </c>
       <c r="AL18" s="124"/>
       <c r="AM18" s="129" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AN18" s="129"/>
       <c r="AO18" s="125"/>
@@ -5767,7 +5764,7 @@
       <c r="D19" s="44"/>
       <c r="E19" s="44"/>
       <c r="F19" s="77" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G19" s="45" t="s">
         <v>25</v>
@@ -5805,11 +5802,11 @@
         <v>34</v>
       </c>
       <c r="T19" s="54" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="U19" s="48"/>
       <c r="V19" s="66" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="W19" s="177">
         <v>40668</v>
@@ -5826,7 +5823,7 @@
         <v>25</v>
       </c>
       <c r="AA19" s="77" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AB19" s="48"/>
       <c r="AC19" s="44"/>
@@ -5845,18 +5842,18 @@
       <c r="AM19" s="49"/>
       <c r="AN19" s="49"/>
       <c r="AO19" s="77" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="20" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" s="42" t="s">
+        <v>468</v>
+      </c>
+      <c r="E20" s="42" t="s">
         <v>469</v>
       </c>
-      <c r="E20" s="42" t="s">
-        <v>470</v>
-      </c>
       <c r="F20" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G20" s="45" t="s">
         <v>25</v>
@@ -5896,7 +5893,7 @@
       </c>
       <c r="U20" s="53"/>
       <c r="V20" s="66" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="W20" s="177"/>
       <c r="X20" s="177"/>
@@ -5926,7 +5923,7 @@
       <c r="AM20" s="54"/>
       <c r="AN20" s="54"/>
       <c r="AO20" s="75" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="21" spans="2:41" s="51" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -5936,10 +5933,10 @@
       </c>
       <c r="D21" s="124"/>
       <c r="E21" s="124" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F21" s="125" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G21" s="203" t="s">
         <v>25</v>
@@ -5973,10 +5970,10 @@
         <v>59</v>
       </c>
       <c r="T21" s="129" t="s">
+        <v>291</v>
+      </c>
+      <c r="U21" s="121" t="s">
         <v>292</v>
-      </c>
-      <c r="U21" s="121" t="s">
-        <v>293</v>
       </c>
       <c r="V21" s="124" t="s">
         <v>218</v>
@@ -5994,7 +5991,7 @@
         <v>0</v>
       </c>
       <c r="AA21" s="125" t="s">
-        <v>291</v>
+        <v>308</v>
       </c>
       <c r="AB21" s="126" t="s">
         <v>25</v>
@@ -6035,7 +6032,7 @@
         <v>157</v>
       </c>
       <c r="F22" s="76" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G22" s="201"/>
       <c r="H22" s="11"/>
@@ -6096,7 +6093,7 @@
       <c r="D23" s="44"/>
       <c r="E23" s="44"/>
       <c r="F23" s="77" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G23" s="45" t="s">
         <v>25</v>
@@ -6131,7 +6128,7 @@
         <v>64</v>
       </c>
       <c r="U23" s="48" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="V23" s="69" t="s">
         <v>219</v>
@@ -6178,7 +6175,7 @@
       <c r="D24" s="44"/>
       <c r="E24" s="44"/>
       <c r="F24" s="77" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G24" s="45" t="s">
         <v>25</v>
@@ -6199,7 +6196,7 @@
         <v>25</v>
       </c>
       <c r="M24" s="46" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="N24" s="47"/>
       <c r="O24" s="109"/>
@@ -6214,10 +6211,10 @@
         <v>204</v>
       </c>
       <c r="T24" s="49" t="s">
+        <v>395</v>
+      </c>
+      <c r="U24" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="U24" s="2" t="s">
-        <v>397</v>
       </c>
       <c r="V24" s="69" t="s">
         <v>222</v>
@@ -6237,7 +6234,7 @@
         <v>13</v>
       </c>
       <c r="AA24" s="77" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB24" s="48" t="s">
         <v>25</v>
@@ -6269,7 +6266,7 @@
       <c r="D25" s="44"/>
       <c r="E25" s="44"/>
       <c r="F25" s="77" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G25" s="45" t="s">
         <v>25</v>
@@ -6286,7 +6283,7 @@
       </c>
       <c r="L25" s="46"/>
       <c r="M25" s="46" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="N25" s="47"/>
       <c r="O25" s="109"/>
@@ -6301,7 +6298,7 @@
         <v>198</v>
       </c>
       <c r="T25" s="49" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="U25" s="48"/>
       <c r="V25" s="69" t="s">
@@ -6320,7 +6317,7 @@
         <v>0</v>
       </c>
       <c r="AA25" s="77" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB25" s="48" t="s">
         <v>25</v>
@@ -6341,11 +6338,11 @@
         <v>25</v>
       </c>
       <c r="AM25" s="49" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AN25" s="49"/>
       <c r="AO25" s="77" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="26" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -6354,10 +6351,10 @@
       </c>
       <c r="D26" s="44"/>
       <c r="E26" s="44" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F26" s="43" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G26" s="45" t="s">
         <v>25</v>
@@ -6376,7 +6373,7 @@
         <v>25</v>
       </c>
       <c r="M26" s="46" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="N26" s="47"/>
       <c r="O26" s="109"/>
@@ -6393,7 +6390,7 @@
       </c>
       <c r="U26" s="48"/>
       <c r="V26" s="153" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="W26" s="179"/>
       <c r="X26" s="179"/>
@@ -6406,7 +6403,7 @@
         <v>0</v>
       </c>
       <c r="AA26" s="77" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB26" s="48"/>
       <c r="AC26" s="44"/>
@@ -6435,10 +6432,10 @@
       </c>
       <c r="D27" s="44"/>
       <c r="E27" s="44" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F27" s="43" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G27" s="45" t="s">
         <v>25</v>
@@ -6464,10 +6461,10 @@
         <v>29</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="S27" s="64" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="T27" s="49" t="s">
         <v>227</v>
@@ -6491,7 +6488,7 @@
         <v>7</v>
       </c>
       <c r="AA27" s="77" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB27" s="48" t="s">
         <v>25</v>
@@ -6520,12 +6517,12 @@
     </row>
     <row r="28" spans="2:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="57" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D28" s="57"/>
       <c r="E28" s="57"/>
       <c r="F28" s="169" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G28" s="58"/>
       <c r="H28" s="58"/>
@@ -6540,7 +6537,7 @@
         <v>25</v>
       </c>
       <c r="M28" s="58" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="N28" s="58"/>
       <c r="O28" s="170"/>
@@ -6549,26 +6546,26 @@
         <v>216</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="S28" s="55" t="s">
+        <v>504</v>
+      </c>
+      <c r="T28" s="57" t="s">
+        <v>502</v>
+      </c>
+      <c r="U28" s="174" t="s">
+        <v>506</v>
+      </c>
+      <c r="V28" s="171" t="s">
         <v>505</v>
-      </c>
-      <c r="T28" s="57" t="s">
-        <v>503</v>
-      </c>
-      <c r="U28" s="174" t="s">
-        <v>507</v>
-      </c>
-      <c r="V28" s="171" t="s">
-        <v>506</v>
       </c>
       <c r="W28" s="185"/>
       <c r="X28" s="185"/>
       <c r="Y28" s="192"/>
       <c r="Z28" s="194"/>
       <c r="AA28" s="57" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB28" s="57"/>
       <c r="AC28" s="57"/>
@@ -6593,7 +6590,7 @@
         <v>211</v>
       </c>
       <c r="F29" s="43" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G29" s="45"/>
       <c r="H29" s="46"/>
@@ -6611,11 +6608,11 @@
       <c r="R29" s="53"/>
       <c r="S29" s="64"/>
       <c r="T29" s="54" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="U29" s="53"/>
       <c r="V29" s="66" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="W29" s="177"/>
       <c r="X29" s="177"/>
@@ -6639,7 +6636,7 @@
         <v>65</v>
       </c>
       <c r="F30" s="75" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G30" s="45" t="s">
         <v>25</v>
@@ -6666,7 +6663,7 @@
         <v>67</v>
       </c>
       <c r="U30" s="53" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="V30" s="65" t="s">
         <v>274</v>
@@ -6686,7 +6683,7 @@
         <v>39</v>
       </c>
       <c r="AA30" s="75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB30" s="53" t="s">
         <v>25</v>
@@ -6710,7 +6707,7 @@
       <c r="AM30" s="54"/>
       <c r="AN30" s="54"/>
       <c r="AO30" s="75" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="31" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -6723,7 +6720,7 @@
         <v>151</v>
       </c>
       <c r="F31" s="77" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G31" s="45" t="s">
         <v>25</v>
@@ -6757,7 +6754,7 @@
       </c>
       <c r="U31" s="48"/>
       <c r="V31" s="153" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="W31" s="179">
         <v>40840</v>
@@ -6774,7 +6771,7 @@
         <v>20</v>
       </c>
       <c r="AA31" s="77" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AB31" s="48"/>
       <c r="AC31" s="44"/>
@@ -6800,7 +6797,7 @@
       </c>
       <c r="C32" s="154"/>
       <c r="F32" s="75" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G32" s="45"/>
       <c r="H32" s="46"/>
@@ -6822,10 +6819,10 @@
       </c>
       <c r="S32" s="64"/>
       <c r="T32" s="54" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="V32" s="66" t="s">
         <v>224</v>
@@ -6867,7 +6864,7 @@
       <c r="D33" s="57"/>
       <c r="E33" s="57"/>
       <c r="F33" s="57" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G33" s="58" t="s">
         <v>25</v>
@@ -6897,7 +6894,7 @@
         <v>72</v>
       </c>
       <c r="T33" s="57" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="U33" s="57"/>
       <c r="V33" s="166">
@@ -6908,7 +6905,7 @@
       <c r="Y33" s="192"/>
       <c r="Z33" s="194"/>
       <c r="AA33" s="57" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="AB33" s="57" t="s">
         <v>25</v>
@@ -6946,7 +6943,7 @@
       <c r="D34" s="51"/>
       <c r="E34" s="51"/>
       <c r="F34" s="158" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G34" s="207" t="s">
         <v>25</v>
@@ -6975,14 +6972,14 @@
         <v>180</v>
       </c>
       <c r="S34" s="216" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="T34" s="160" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="U34" s="159"/>
       <c r="V34" s="217" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="W34" s="183"/>
       <c r="X34" s="183">
@@ -6997,7 +6994,7 @@
         <v>0</v>
       </c>
       <c r="AA34" s="158" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB34" s="159" t="s">
         <v>25</v>
@@ -7029,10 +7026,10 @@
         <v>74</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F35" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G35" s="45" t="s">
         <v>25</v>
@@ -7059,7 +7056,7 @@
       <c r="S35" s="64"/>
       <c r="T35" s="54"/>
       <c r="U35" s="53" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="V35" s="163">
         <v>40756</v>
@@ -7077,7 +7074,7 @@
         <v>23</v>
       </c>
       <c r="AA35" s="75" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AB35" s="53"/>
       <c r="AG35" s="54"/>
@@ -7095,7 +7092,7 @@
       <c r="AM35" s="54"/>
       <c r="AN35" s="54"/>
       <c r="AO35" s="75" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="36" spans="2:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -7106,7 +7103,7 @@
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="74" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>25</v>
@@ -7124,13 +7121,13 @@
         <v>29</v>
       </c>
       <c r="R36" s="164" t="s">
+        <v>465</v>
+      </c>
+      <c r="S36" s="61" t="s">
         <v>466</v>
       </c>
-      <c r="S36" s="61" t="s">
+      <c r="T36" s="23" t="s">
         <v>467</v>
-      </c>
-      <c r="T36" s="23" t="s">
-        <v>468</v>
       </c>
       <c r="U36" s="22"/>
       <c r="V36" s="62">
@@ -7171,7 +7168,7 @@
         <v>76</v>
       </c>
       <c r="F37" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G37" s="45" t="s">
         <v>25</v>
@@ -7194,16 +7191,16 @@
         <v>77</v>
       </c>
       <c r="S37" s="64" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="T37" s="54" t="s">
         <v>79</v>
       </c>
       <c r="U37" s="53" t="s">
+        <v>463</v>
+      </c>
+      <c r="V37" s="163" t="s">
         <v>464</v>
-      </c>
-      <c r="V37" s="163" t="s">
-        <v>465</v>
       </c>
       <c r="W37" s="177">
         <v>41331</v>
@@ -7218,7 +7215,7 @@
         <v>4</v>
       </c>
       <c r="AA37" s="75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB37" s="53"/>
       <c r="AG37" s="54"/>
@@ -7239,13 +7236,13 @@
     </row>
     <row r="38" spans="2:41" s="63" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="76" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G38" s="201"/>
       <c r="H38" s="11"/>
@@ -7263,15 +7260,15 @@
         <v>216</v>
       </c>
       <c r="R38" s="32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="S38" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="T38" s="33"/>
       <c r="U38" s="34"/>
       <c r="V38" s="143" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="W38" s="178">
         <v>40443</v>
@@ -7296,15 +7293,15 @@
       <c r="AM38" s="33"/>
       <c r="AN38" s="33"/>
       <c r="AO38" s="76" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="39" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="44" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F39" s="75" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G39" s="45"/>
       <c r="H39" s="46"/>
@@ -7322,15 +7319,15 @@
         <v>78</v>
       </c>
       <c r="R39" s="173" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S39" s="64"/>
       <c r="T39" s="54" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="U39" s="48"/>
       <c r="V39" s="65" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="W39" s="177">
         <v>41061</v>
@@ -7364,7 +7361,7 @@
       <c r="D40" s="42"/>
       <c r="E40" s="42"/>
       <c r="F40" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G40" s="45" t="s">
         <v>25</v>
@@ -7390,7 +7387,7 @@
       </c>
       <c r="O40" s="110"/>
       <c r="P40" s="103" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="Q40" s="54" t="s">
         <v>29</v>
@@ -7402,10 +7399,10 @@
         <v>82</v>
       </c>
       <c r="T40" s="54" t="s">
+        <v>301</v>
+      </c>
+      <c r="U40" s="53" t="s">
         <v>302</v>
-      </c>
-      <c r="U40" s="53" t="s">
-        <v>303</v>
       </c>
       <c r="V40" s="66" t="s">
         <v>207</v>
@@ -7425,7 +7422,7 @@
         <v>30</v>
       </c>
       <c r="AA40" s="75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB40" s="53" t="s">
         <v>25</v>
@@ -7460,7 +7457,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="78" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G41" s="18" t="s">
         <v>25</v>
@@ -7499,10 +7496,10 @@
         <v>83</v>
       </c>
       <c r="U41" s="172" t="s">
+        <v>412</v>
+      </c>
+      <c r="V41" s="67" t="s">
         <v>413</v>
-      </c>
-      <c r="V41" s="67" t="s">
-        <v>414</v>
       </c>
       <c r="W41" s="186">
         <v>40878</v>
@@ -7545,7 +7542,7 @@
       <c r="AM41" s="31"/>
       <c r="AN41" s="31"/>
       <c r="AO41" s="74" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="42" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -7553,10 +7550,10 @@
         <v>251</v>
       </c>
       <c r="E42" s="44" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F42" s="77" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G42" s="45" t="s">
         <v>31</v>
@@ -7567,7 +7564,7 @@
       <c r="K42" s="46"/>
       <c r="L42" s="46"/>
       <c r="M42" s="46" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="N42" s="47"/>
       <c r="O42" s="88"/>
@@ -7579,16 +7576,16 @@
         <v>252</v>
       </c>
       <c r="S42" s="64" t="s">
+        <v>409</v>
+      </c>
+      <c r="T42" s="54" t="s">
+        <v>407</v>
+      </c>
+      <c r="U42" s="53" t="s">
         <v>410</v>
       </c>
-      <c r="T42" s="54" t="s">
-        <v>408</v>
-      </c>
-      <c r="U42" s="53" t="s">
+      <c r="V42" s="65" t="s">
         <v>411</v>
-      </c>
-      <c r="V42" s="65" t="s">
-        <v>412</v>
       </c>
       <c r="W42" s="177"/>
       <c r="X42" s="177">
@@ -7603,7 +7600,7 @@
         <v>0</v>
       </c>
       <c r="AA42" s="77" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB42" s="48" t="s">
         <v>25</v>
@@ -7631,7 +7628,7 @@
       <c r="D43" s="115"/>
       <c r="E43" s="115"/>
       <c r="F43" s="116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G43" s="133"/>
       <c r="H43" s="134"/>
@@ -7658,16 +7655,16 @@
         <v>87</v>
       </c>
       <c r="S43" s="122" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="T43" s="120" t="s">
+        <v>362</v>
+      </c>
+      <c r="U43" s="121" t="s">
         <v>363</v>
       </c>
-      <c r="U43" s="121" t="s">
-        <v>364</v>
-      </c>
       <c r="V43" s="144" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="W43" s="175"/>
       <c r="X43" s="175">
@@ -7682,7 +7679,7 @@
         <v>0</v>
       </c>
       <c r="AA43" s="116" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB43" s="121" t="s">
         <v>25</v>
@@ -7716,7 +7713,7 @@
       </c>
       <c r="AN43" s="120"/>
       <c r="AO43" s="116" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="44" spans="2:41" s="63" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -7727,7 +7724,7 @@
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="76" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G44" s="201"/>
       <c r="H44" s="11"/>
@@ -7741,7 +7738,7 @@
       <c r="N44" s="202"/>
       <c r="O44" s="89"/>
       <c r="P44" s="102" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Q44" s="33" t="s">
         <v>216</v>
@@ -7750,12 +7747,12 @@
         <v>89</v>
       </c>
       <c r="S44" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="T44" s="33"/>
       <c r="U44" s="24"/>
       <c r="V44" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="W44" s="178"/>
       <c r="X44" s="178"/>
@@ -7786,10 +7783,10 @@
         <v>90</v>
       </c>
       <c r="E45" s="42" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F45" s="75" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G45" s="45"/>
       <c r="H45" s="46"/>
@@ -7798,7 +7795,7 @@
       <c r="K45" s="46"/>
       <c r="L45" s="46"/>
       <c r="M45" s="46" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="N45" s="47"/>
       <c r="O45" s="110"/>
@@ -7817,7 +7814,7 @@
       </c>
       <c r="U45" s="52"/>
       <c r="V45" s="66" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="W45" s="177"/>
       <c r="X45" s="177">
@@ -7832,7 +7829,7 @@
         <v>0</v>
       </c>
       <c r="AA45" s="75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB45" s="53"/>
       <c r="AG45" s="54"/>
@@ -7855,7 +7852,7 @@
       <c r="D46" s="115"/>
       <c r="E46" s="115"/>
       <c r="F46" s="116" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G46" s="133"/>
       <c r="H46" s="134"/>
@@ -7882,7 +7879,7 @@
         <v>238</v>
       </c>
       <c r="U46" s="121" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="V46" s="123" t="s">
         <v>237</v>
@@ -7902,7 +7899,7 @@
         <v>10</v>
       </c>
       <c r="AA46" s="132" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB46" s="138"/>
       <c r="AC46" s="131"/>
@@ -7935,7 +7932,7 @@
       <c r="D47" s="115"/>
       <c r="E47" s="115"/>
       <c r="F47" s="116" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G47" s="133"/>
       <c r="H47" s="134"/>
@@ -7956,13 +7953,13 @@
         <v>95</v>
       </c>
       <c r="S47" s="122" t="s">
+        <v>332</v>
+      </c>
+      <c r="T47" s="120" t="s">
+        <v>331</v>
+      </c>
+      <c r="U47" s="121" t="s">
         <v>333</v>
-      </c>
-      <c r="T47" s="120" t="s">
-        <v>332</v>
-      </c>
-      <c r="U47" s="121" t="s">
-        <v>334</v>
       </c>
       <c r="V47" s="141" t="s">
         <v>208</v>
@@ -7975,14 +7972,14 @@
       </c>
       <c r="Y47" s="192">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Z47" s="194">
         <f t="shared" ca="1" si="3"/>
         <v>29</v>
       </c>
       <c r="AA47" s="116" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB47" s="121" t="s">
         <v>25</v>
@@ -8002,20 +7999,20 @@
       </c>
       <c r="AL47" s="115"/>
       <c r="AM47" s="120" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AN47" s="120"/>
       <c r="AO47" s="116"/>
     </row>
     <row r="48" spans="2:41" s="51" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="124" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C48" s="124"/>
       <c r="D48" s="124"/>
       <c r="E48" s="124"/>
       <c r="F48" s="125" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G48" s="203" t="s">
         <v>25</v>
@@ -8030,7 +8027,7 @@
       <c r="K48" s="204"/>
       <c r="L48" s="204"/>
       <c r="M48" s="204" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N48" s="205"/>
       <c r="O48" s="127"/>
@@ -8048,7 +8045,7 @@
         <v>97</v>
       </c>
       <c r="U48" s="121" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="V48" s="124" t="s">
         <v>191</v>
@@ -8068,7 +8065,7 @@
         <v>62</v>
       </c>
       <c r="AA48" s="125" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB48" s="126" t="s">
         <v>25</v>
@@ -8092,10 +8089,10 @@
       </c>
       <c r="AL48" s="124"/>
       <c r="AM48" s="129" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AN48" s="129" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AO48" s="125"/>
     </row>
@@ -8107,7 +8104,7 @@
       <c r="D49" s="124"/>
       <c r="E49" s="124"/>
       <c r="F49" s="125" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G49" s="203" t="s">
         <v>25</v>
@@ -8126,7 +8123,7 @@
         <v>25</v>
       </c>
       <c r="M49" s="204" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="N49" s="205" t="s">
         <v>25</v>
@@ -8145,7 +8142,7 @@
         <v>197</v>
       </c>
       <c r="T49" s="129" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="U49" s="126" t="s">
         <v>192</v>
@@ -8168,7 +8165,7 @@
         <v>68</v>
       </c>
       <c r="AA49" s="150" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB49" s="126" t="s">
         <v>25</v>
@@ -8204,10 +8201,10 @@
       <c r="C50" s="44"/>
       <c r="D50" s="44"/>
       <c r="E50" s="44" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F50" s="77" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G50" s="45"/>
       <c r="H50" s="46" t="s">
@@ -8231,13 +8228,13 @@
         <v>102</v>
       </c>
       <c r="T50" s="49" t="s">
+        <v>430</v>
+      </c>
+      <c r="U50" s="45" t="s">
         <v>431</v>
       </c>
-      <c r="U50" s="45" t="s">
-        <v>432</v>
-      </c>
       <c r="V50" s="157" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="W50" s="179">
         <v>40865</v>
@@ -8247,14 +8244,14 @@
       </c>
       <c r="Y50" s="192">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Z50" s="194">
         <f t="shared" ca="1" si="3"/>
         <v>19</v>
       </c>
       <c r="AA50" s="77" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AB50" s="48" t="s">
         <v>25</v>
@@ -8273,7 +8270,7 @@
       <c r="AM50" s="49"/>
       <c r="AN50" s="49"/>
       <c r="AO50" s="75" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="51" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -8281,7 +8278,7 @@
         <v>103</v>
       </c>
       <c r="F51" s="75" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G51" s="45" t="s">
         <v>25</v>
@@ -8310,7 +8307,7 @@
         <v>103</v>
       </c>
       <c r="U51" s="52" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="V51" s="66" t="s">
         <v>209</v>
@@ -8330,7 +8327,7 @@
         <v>23</v>
       </c>
       <c r="AA51" s="75" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AB51" s="53" t="s">
         <v>25</v>
@@ -8358,7 +8355,7 @@
         <v>25</v>
       </c>
       <c r="AM51" s="54" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AN51" s="54"/>
       <c r="AO51" s="75" t="s">
@@ -8370,14 +8367,14 @@
         <v>256</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D52" s="44"/>
       <c r="E52" s="44" t="s">
+        <v>438</v>
+      </c>
+      <c r="F52" s="77" t="s">
         <v>439</v>
-      </c>
-      <c r="F52" s="77" t="s">
-        <v>440</v>
       </c>
       <c r="G52" s="45" t="s">
         <v>25</v>
@@ -8395,15 +8392,15 @@
         <v>29</v>
       </c>
       <c r="R52" s="48" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="S52" s="64"/>
       <c r="T52" s="54" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="U52" s="53"/>
       <c r="V52" s="66" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="W52" s="177">
         <v>39249</v>
@@ -8420,7 +8417,7 @@
         <v>72</v>
       </c>
       <c r="AA52" s="77" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB52" s="53" t="s">
         <v>25</v>
@@ -8439,7 +8436,7 @@
       <c r="AM52" s="54"/>
       <c r="AN52" s="54"/>
       <c r="AO52" s="75" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="53" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -8450,7 +8447,7 @@
       <c r="D53" s="44"/>
       <c r="E53" s="44"/>
       <c r="F53" s="77" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G53" s="45" t="s">
         <v>25</v>
@@ -8471,13 +8468,13 @@
         <v>171</v>
       </c>
       <c r="S53" s="64" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="T53" s="54" t="s">
         <v>170</v>
       </c>
       <c r="U53" s="53" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="V53" s="66">
         <v>2005</v>
@@ -8508,18 +8505,18 @@
       <c r="AM53" s="54"/>
       <c r="AN53" s="54"/>
       <c r="AO53" s="75" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="54" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="131" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C54" s="131"/>
       <c r="D54" s="131"/>
       <c r="E54" s="131"/>
       <c r="F54" s="132" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G54" s="133" t="s">
         <v>25</v>
@@ -8574,7 +8571,7 @@
         <v>56</v>
       </c>
       <c r="AA54" s="132" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB54" s="121" t="s">
         <v>25</v>
@@ -8602,7 +8599,7 @@
       </c>
       <c r="AL54" s="115"/>
       <c r="AM54" s="120" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AN54" s="120"/>
       <c r="AO54" s="116"/>
@@ -8615,7 +8612,7 @@
       <c r="D55" s="44"/>
       <c r="E55" s="44"/>
       <c r="F55" s="77" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G55" s="45"/>
       <c r="H55" s="46" t="s">
@@ -8643,7 +8640,7 @@
       </c>
       <c r="U55" s="45"/>
       <c r="V55" s="66" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="W55" s="177"/>
       <c r="X55" s="177"/>
@@ -8678,7 +8675,7 @@
         <v>112</v>
       </c>
       <c r="F56" s="75" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G56" s="45" t="s">
         <v>25</v>
@@ -8719,7 +8716,7 @@
         <v>22</v>
       </c>
       <c r="AA56" s="75" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AB56" s="53"/>
       <c r="AG56" s="54"/>
@@ -8745,10 +8742,10 @@
         <v>163</v>
       </c>
       <c r="E57" s="42" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F57" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G57" s="45"/>
       <c r="H57" s="46"/>
@@ -8763,7 +8760,7 @@
         <v>25</v>
       </c>
       <c r="M57" s="46" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N57" s="47"/>
       <c r="O57" s="110"/>
@@ -8774,19 +8771,19 @@
         <v>78</v>
       </c>
       <c r="R57" s="173" t="s">
+        <v>449</v>
+      </c>
+      <c r="S57" s="64" t="s">
+        <v>451</v>
+      </c>
+      <c r="T57" s="54" t="s">
         <v>450</v>
       </c>
-      <c r="S57" s="64" t="s">
+      <c r="U57" s="53" t="s">
         <v>452</v>
       </c>
-      <c r="T57" s="54" t="s">
-        <v>451</v>
-      </c>
-      <c r="U57" s="53" t="s">
-        <v>453</v>
-      </c>
       <c r="V57" s="65" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="W57" s="177">
         <v>41080</v>
@@ -8801,7 +8798,7 @@
         <v>12</v>
       </c>
       <c r="AA57" s="75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB57" s="53" t="s">
         <v>25</v>
@@ -8837,7 +8834,7 @@
       <c r="D58" s="115"/>
       <c r="E58" s="115"/>
       <c r="F58" s="116" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G58" s="133"/>
       <c r="H58" s="134"/>
@@ -8860,16 +8857,16 @@
         <v>118</v>
       </c>
       <c r="S58" s="122" t="s">
+        <v>305</v>
+      </c>
+      <c r="T58" s="54" t="s">
         <v>306</v>
       </c>
-      <c r="T58" s="54" t="s">
+      <c r="U58" s="53" t="s">
         <v>307</v>
       </c>
-      <c r="U58" s="53" t="s">
-        <v>308</v>
-      </c>
       <c r="V58" s="144" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="W58" s="175">
         <v>41099</v>
@@ -8886,7 +8883,7 @@
         <v>11</v>
       </c>
       <c r="AA58" s="116" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB58" s="121" t="s">
         <v>25</v>
@@ -8908,7 +8905,7 @@
       </c>
       <c r="AL58" s="115"/>
       <c r="AM58" s="120" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AN58" s="120"/>
       <c r="AO58" s="116"/>
@@ -8918,10 +8915,10 @@
         <v>119</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G59" s="58"/>
       <c r="H59" s="58"/>
@@ -8942,10 +8939,10 @@
       </c>
       <c r="S59" s="55"/>
       <c r="T59" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="V59" s="56" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="W59" s="184"/>
       <c r="X59" s="184"/>
@@ -8959,10 +8956,10 @@
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F60" s="76" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G60" s="201"/>
       <c r="H60" s="11"/>
@@ -8984,11 +8981,11 @@
       </c>
       <c r="S60" s="12"/>
       <c r="T60" s="33" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="U60" s="32"/>
       <c r="V60" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="W60" s="178"/>
       <c r="X60" s="178"/>
@@ -9015,18 +9012,18 @@
       <c r="AM60" s="33"/>
       <c r="AN60" s="33"/>
       <c r="AO60" s="76" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="61" spans="2:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G61" s="58"/>
       <c r="H61" s="58"/>
@@ -9051,7 +9048,7 @@
       </c>
       <c r="U61" s="167"/>
       <c r="V61" s="56" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="W61" s="184"/>
       <c r="X61" s="184"/>
@@ -9063,7 +9060,7 @@
         <v>123</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G62" s="58"/>
       <c r="H62" s="58"/>
@@ -9083,10 +9080,10 @@
         <v>124</v>
       </c>
       <c r="S62" s="55" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="V62" s="56" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="W62" s="184"/>
       <c r="X62" s="184"/>
@@ -9102,10 +9099,10 @@
       </c>
       <c r="D63" s="115"/>
       <c r="E63" s="115" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F63" s="116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G63" s="133" t="s">
         <v>25</v>
@@ -9135,7 +9132,7 @@
         <v>29</v>
       </c>
       <c r="R63" s="148" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S63" s="122" t="s">
         <v>202</v>
@@ -9162,7 +9159,7 @@
         <v>25</v>
       </c>
       <c r="AA63" s="116" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AB63" s="121" t="s">
         <v>25</v>
@@ -9188,18 +9185,18 @@
       <c r="AM63" s="120"/>
       <c r="AN63" s="120"/>
       <c r="AO63" s="116" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="64" spans="2:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
       <c r="F64" s="74" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G64" s="18" t="s">
         <v>25</v>
@@ -9238,7 +9235,7 @@
         <v>0</v>
       </c>
       <c r="AA64" s="74" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AB64" s="22"/>
       <c r="AC64" s="10"/>
@@ -9267,7 +9264,7 @@
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
       <c r="F65" s="74" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G65" s="18" t="s">
         <v>31</v>
@@ -9294,7 +9291,7 @@
         <v>261</v>
       </c>
       <c r="U65" s="22" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="V65" s="62"/>
       <c r="W65" s="181"/>
@@ -9335,10 +9332,10 @@
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F66" s="76" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G66" s="201"/>
       <c r="H66" s="11"/>
@@ -9359,14 +9356,14 @@
         <v>135</v>
       </c>
       <c r="S66" s="12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="T66" s="33" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="U66" s="32"/>
       <c r="V66" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="W66" s="178">
         <v>40609</v>
@@ -9377,7 +9374,7 @@
       <c r="Y66" s="192"/>
       <c r="Z66" s="194"/>
       <c r="AA66" s="76" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB66" s="32" t="s">
         <v>25</v>
@@ -9408,7 +9405,7 @@
         <v>160</v>
       </c>
       <c r="F67" s="116" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G67" s="133"/>
       <c r="H67" s="134"/>
@@ -9432,7 +9429,7 @@
         <v>246</v>
       </c>
       <c r="T67" s="120" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="U67" s="121"/>
       <c r="V67" s="141" t="s">
@@ -9453,7 +9450,7 @@
         <v>26</v>
       </c>
       <c r="AA67" s="116" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AB67" s="121" t="s">
         <v>25</v>
@@ -9475,11 +9472,11 @@
       </c>
       <c r="AL67" s="115"/>
       <c r="AM67" s="120" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AN67" s="120"/>
       <c r="AO67" s="116" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="68" spans="1:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9487,10 +9484,10 @@
         <v>132</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G68" s="58"/>
       <c r="H68" s="58"/>
@@ -9510,10 +9507,10 @@
         <v>133</v>
       </c>
       <c r="S68" s="55" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="V68" s="56" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="W68" s="184"/>
       <c r="X68" s="184"/>
@@ -9525,13 +9522,13 @@
     </row>
     <row r="69" spans="1:41" s="51" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B69" s="124" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C69" s="124"/>
       <c r="D69" s="124"/>
       <c r="E69" s="124"/>
       <c r="F69" s="125" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G69" s="203"/>
       <c r="H69" s="204"/>
@@ -9555,7 +9552,7 @@
         <v>241</v>
       </c>
       <c r="T69" s="129" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="U69" s="126"/>
       <c r="V69" s="124" t="s">
@@ -9604,10 +9601,10 @@
       <c r="C70" s="115"/>
       <c r="D70" s="115"/>
       <c r="E70" s="115" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F70" s="116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G70" s="133"/>
       <c r="H70" s="134"/>
@@ -9624,7 +9621,7 @@
         <v>25</v>
       </c>
       <c r="M70" s="134" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N70" s="135" t="s">
         <v>25</v>
@@ -9640,16 +9637,16 @@
         <v>234</v>
       </c>
       <c r="S70" s="122" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="T70" s="120" t="s">
         <v>233</v>
       </c>
       <c r="U70" s="121" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="V70" s="123" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="W70" s="175"/>
       <c r="X70" s="175"/>
@@ -9662,7 +9659,7 @@
         <v>0</v>
       </c>
       <c r="AA70" s="132" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB70" s="138" t="s">
         <v>25</v>
@@ -9690,7 +9687,7 @@
         <v>136</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G71" s="58"/>
       <c r="H71" s="58"/>
@@ -9710,7 +9707,7 @@
         <v>137</v>
       </c>
       <c r="S71" s="55" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="V71" s="56"/>
       <c r="W71" s="184"/>
@@ -9732,7 +9729,7 @@
         <v>44</v>
       </c>
       <c r="F72" s="75" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G72" s="45"/>
       <c r="H72" s="46"/>
@@ -9753,14 +9750,14 @@
         <v>139</v>
       </c>
       <c r="S72" s="64" t="s">
+        <v>414</v>
+      </c>
+      <c r="T72" s="54" t="s">
         <v>415</v>
-      </c>
-      <c r="T72" s="54" t="s">
-        <v>416</v>
       </c>
       <c r="U72" s="53"/>
       <c r="V72" s="66" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="W72" s="177">
         <v>40561</v>
@@ -9800,7 +9797,7 @@
       </c>
       <c r="E73" s="44"/>
       <c r="F73" s="77" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G73" s="45"/>
       <c r="H73" s="46"/>
@@ -9843,7 +9840,7 @@
         <v>28</v>
       </c>
       <c r="AA73" s="77" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB73" s="48"/>
       <c r="AC73" s="44"/>
@@ -9875,10 +9872,10 @@
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
       <c r="E74" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F74" s="74" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G74" s="18" t="s">
         <v>25</v>
@@ -9899,16 +9896,16 @@
         <v>173</v>
       </c>
       <c r="S74" s="61" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="T74" s="23" t="s">
         <v>116</v>
       </c>
       <c r="U74" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="V74" s="62" t="s">
         <v>512</v>
-      </c>
-      <c r="V74" s="62" t="s">
-        <v>513</v>
       </c>
       <c r="W74" s="181">
         <v>40940</v>
@@ -9925,7 +9922,7 @@
         <v>17</v>
       </c>
       <c r="AA74" s="74" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB74" s="22"/>
       <c r="AC74" s="10"/>
@@ -9948,10 +9945,10 @@
     </row>
     <row r="75" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="42" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F75" s="75" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G75" s="45" t="s">
         <v>25</v>
@@ -9971,7 +9968,7 @@
         <v>29</v>
       </c>
       <c r="R75" s="53" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="S75" s="64"/>
       <c r="T75" s="54" t="s">
@@ -9979,7 +9976,7 @@
       </c>
       <c r="U75" s="53"/>
       <c r="V75" s="65" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="W75" s="177">
         <v>40828</v>
@@ -9996,7 +9993,7 @@
         <v>20</v>
       </c>
       <c r="AA75" s="75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB75" s="53" t="s">
         <v>25</v>
@@ -10030,10 +10027,10 @@
         <v>253</v>
       </c>
       <c r="E76" s="44" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F76" s="77" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G76" s="45"/>
       <c r="H76" s="46" t="s">
@@ -10097,7 +10094,7 @@
         <v>177</v>
       </c>
       <c r="F77" s="75" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G77" s="45"/>
       <c r="H77" s="46"/>
@@ -10120,7 +10117,7 @@
         <v>178</v>
       </c>
       <c r="S77" s="64" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="T77" s="54" t="s">
         <v>177</v>
@@ -10142,7 +10139,7 @@
         <v>0</v>
       </c>
       <c r="AA77" s="75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB77" s="53" t="s">
         <v>25</v>
@@ -10161,7 +10158,7 @@
       <c r="AM77" s="54"/>
       <c r="AN77" s="54"/>
       <c r="AO77" s="75" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="78" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10172,7 +10169,7 @@
         <v>161</v>
       </c>
       <c r="F78" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G78" s="45" t="s">
         <v>25</v>
@@ -10202,11 +10199,11 @@
         <v>145</v>
       </c>
       <c r="T78" s="54" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="U78" s="53"/>
       <c r="V78" s="65" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W78" s="177">
         <v>40252</v>
@@ -10221,7 +10218,7 @@
         <v>39</v>
       </c>
       <c r="AA78" s="75" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AB78" s="53" t="s">
         <v>25</v>
@@ -10251,7 +10248,7 @@
       <c r="AM78" s="54"/>
       <c r="AN78" s="54"/>
       <c r="AO78" s="75" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="79" spans="1:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10259,10 +10256,10 @@
         <v>239</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G79" s="58" t="s">
         <v>25</v>
@@ -10312,7 +10309,7 @@
       <c r="D80" s="131"/>
       <c r="E80" s="131"/>
       <c r="F80" s="132" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G80" s="133"/>
       <c r="H80" s="134"/>
@@ -10381,10 +10378,10 @@
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F81" s="76" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G81" s="201" t="s">
         <v>25</v>
@@ -10441,7 +10438,7 @@
       <c r="AM81" s="33"/>
       <c r="AN81" s="33"/>
       <c r="AO81" s="76" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -10449,7 +10446,7 @@
         <v>164</v>
       </c>
       <c r="F82" s="75" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G82" s="45" t="s">
         <v>25</v>
@@ -10463,7 +10460,7 @@
       <c r="N82" s="47"/>
       <c r="O82" s="110"/>
       <c r="P82" s="103" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="Q82" s="54" t="s">
         <v>29</v>
@@ -10473,7 +10470,7 @@
       </c>
       <c r="S82" s="64"/>
       <c r="T82" s="54" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="U82" s="53"/>
       <c r="V82" s="66"/>
@@ -10488,7 +10485,7 @@
         <v>0</v>
       </c>
       <c r="AA82" s="77" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AB82" s="48"/>
       <c r="AC82" s="44"/>
@@ -10513,7 +10510,7 @@
         <v>176</v>
       </c>
       <c r="F83" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G83" s="45" t="s">
         <v>25</v>
@@ -10530,7 +10527,7 @@
       </c>
       <c r="L83" s="46"/>
       <c r="M83" s="46" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N83" s="47"/>
       <c r="O83" s="110"/>
@@ -10543,7 +10540,7 @@
       </c>
       <c r="S83" s="64"/>
       <c r="T83" s="54" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="U83" s="53"/>
       <c r="V83" s="66"/>
@@ -10558,7 +10555,7 @@
         <v>0</v>
       </c>
       <c r="AA83" s="75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB83" s="53" t="s">
         <v>25</v>
@@ -10578,7 +10575,7 @@
         <v>271</v>
       </c>
       <c r="F84" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G84" s="45"/>
       <c r="H84" s="46"/>
@@ -10605,16 +10602,16 @@
         <v>272</v>
       </c>
       <c r="S84" s="64" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="T84" s="54" t="s">
         <v>273</v>
       </c>
       <c r="U84" s="53" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="V84" s="66" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="W84" s="177">
         <v>39794</v>
@@ -10631,7 +10628,7 @@
         <v>54</v>
       </c>
       <c r="AA84" s="75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB84" s="53" t="s">
         <v>25</v>
@@ -10645,15 +10642,15 @@
       <c r="AM84" s="54"/>
       <c r="AN84" s="54"/>
       <c r="AO84" s="75" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="85" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="42" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F85" s="75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G85" s="45"/>
       <c r="H85" s="46"/>
@@ -10673,7 +10670,7 @@
         <v>78</v>
       </c>
       <c r="R85" s="53" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="S85" s="64" t="s">
         <v>147</v>
@@ -10682,10 +10679,10 @@
         <v>148</v>
       </c>
       <c r="U85" s="53" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="V85" s="163" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="W85" s="177">
         <v>40497</v>
@@ -10716,7 +10713,7 @@
       <c r="AM85" s="54"/>
       <c r="AN85" s="54"/>
       <c r="AO85" s="75" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="86" spans="2:41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
. = _ in names, eol folder
</commit_message>
<xml_diff>
--- a/Cloud Platforms (PaaS).xlsx
+++ b/Cloud Platforms (PaaS).xlsx
@@ -1435,9 +1435,6 @@
     <t>@appfog</t>
   </si>
   <si>
-    <t>PHP Fog (AppFog)</t>
-  </si>
-  <si>
     <t>https://www.phpfog.com/</t>
   </si>
   <si>
@@ -2873,6 +2870,9 @@
   </si>
   <si>
     <t>Opa</t>
+  </si>
+  <si>
+    <t>PHP Fog</t>
   </si>
 </sst>
 </file>
@@ -4222,10 +4222,10 @@
   <dimension ref="A1:AO320"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="S16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="S19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AA21" sqref="AA21"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4286,7 +4286,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="112" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G1" s="224" t="s">
         <v>4</v>
@@ -4299,7 +4299,7 @@
       <c r="M1" s="225"/>
       <c r="N1" s="227"/>
       <c r="O1" s="107" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="P1" s="98" t="s">
         <v>5</v>
@@ -4317,19 +4317,19 @@
         <v>9</v>
       </c>
       <c r="U1" s="82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="V1" s="83" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="W1" s="180" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X1" s="180" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="Y1" s="235" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Z1" s="236"/>
       <c r="AA1" s="73" t="s">
@@ -4344,17 +4344,17 @@
       <c r="AF1" s="230"/>
       <c r="AG1" s="231"/>
       <c r="AH1" s="221" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AI1" s="222"/>
       <c r="AJ1" s="223"/>
       <c r="AK1" s="221" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AL1" s="222"/>
       <c r="AM1" s="223"/>
       <c r="AN1" s="220" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AO1" s="73" t="s">
         <v>12</v>
@@ -4362,7 +4362,7 @@
     </row>
     <row r="2" spans="1:41" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="232" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C2" s="232"/>
       <c r="D2" s="232"/>
@@ -4387,10 +4387,10 @@
         <v>19</v>
       </c>
       <c r="M2" s="197" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N2" s="200" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O2" s="85"/>
       <c r="P2" s="99"/>
@@ -4406,14 +4406,14 @@
         <v>29</v>
       </c>
       <c r="Z2" s="189" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AA2" s="74"/>
       <c r="AB2" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="AC2" s="6" t="s">
         <v>349</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>350</v>
       </c>
       <c r="AD2" s="6" t="s">
         <v>20</v>
@@ -4425,25 +4425,25 @@
         <v>22</v>
       </c>
       <c r="AG2" s="31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AH2" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="AI2" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="31" t="s">
         <v>278</v>
       </c>
-      <c r="AJ2" s="31" t="s">
-        <v>279</v>
-      </c>
       <c r="AK2" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="AL2" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="AL2" s="6" t="s">
-        <v>284</v>
-      </c>
       <c r="AM2" s="31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AN2" s="31"/>
       <c r="AO2" s="74"/>
@@ -4563,13 +4563,13 @@
     </row>
     <row r="4" spans="1:41" s="63" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="76" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G4" s="201"/>
       <c r="H4" s="11"/>
@@ -4584,20 +4584,20 @@
       <c r="O4" s="89"/>
       <c r="P4" s="102"/>
       <c r="Q4" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R4" s="147" t="s">
         <v>26</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T4" s="33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="U4" s="32"/>
       <c r="V4" s="114" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="W4" s="178">
         <v>40878</v>
@@ -4622,7 +4622,7 @@
       <c r="AM4" s="33"/>
       <c r="AN4" s="33"/>
       <c r="AO4" s="76" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -4632,10 +4632,10 @@
       <c r="C5" s="115"/>
       <c r="D5" s="115"/>
       <c r="E5" s="115" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F5" s="116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G5" s="133"/>
       <c r="H5" s="134"/>
@@ -4649,7 +4649,7 @@
       <c r="N5" s="135"/>
       <c r="O5" s="118"/>
       <c r="P5" s="119" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="Q5" s="120" t="s">
         <v>29</v>
@@ -4658,16 +4658,16 @@
         <v>28</v>
       </c>
       <c r="S5" s="122" t="s">
+        <v>383</v>
+      </c>
+      <c r="T5" s="120" t="s">
         <v>384</v>
       </c>
-      <c r="T5" s="120" t="s">
+      <c r="U5" s="117" t="s">
         <v>385</v>
       </c>
-      <c r="U5" s="117" t="s">
+      <c r="V5" s="123" t="s">
         <v>386</v>
-      </c>
-      <c r="V5" s="123" t="s">
-        <v>387</v>
       </c>
       <c r="W5" s="175"/>
       <c r="X5" s="175">
@@ -4682,7 +4682,7 @@
         <v>0</v>
       </c>
       <c r="AA5" s="116" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB5" s="121" t="s">
         <v>25</v>
@@ -4725,7 +4725,7 @@
       <c r="D6" s="124"/>
       <c r="E6" s="124"/>
       <c r="F6" s="125" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G6" s="203" t="s">
         <v>25</v>
@@ -4750,22 +4750,22 @@
       <c r="O6" s="127"/>
       <c r="P6" s="128"/>
       <c r="Q6" s="129" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R6" s="126" t="s">
         <v>36</v>
       </c>
       <c r="S6" s="130" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="T6" s="129" t="s">
         <v>30</v>
       </c>
       <c r="U6" s="126" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="V6" s="124" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W6" s="176">
         <v>40562</v>
@@ -4780,7 +4780,7 @@
         <v>29</v>
       </c>
       <c r="AA6" s="125" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB6" s="126" t="s">
         <v>25</v>
@@ -4812,7 +4812,7 @@
       </c>
       <c r="AL6" s="124"/>
       <c r="AM6" s="129" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AN6" s="129"/>
       <c r="AO6" s="125"/>
@@ -4825,7 +4825,7 @@
       <c r="D7" s="131"/>
       <c r="E7" s="131"/>
       <c r="F7" s="132" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G7" s="133"/>
       <c r="H7" s="134" t="s">
@@ -4841,7 +4841,7 @@
         <v>25</v>
       </c>
       <c r="P7" s="137" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q7" s="120" t="s">
         <v>29</v>
@@ -4850,16 +4850,16 @@
         <v>38</v>
       </c>
       <c r="S7" s="122" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T7" s="120" t="s">
+        <v>288</v>
+      </c>
+      <c r="U7" s="121" t="s">
         <v>289</v>
       </c>
-      <c r="U7" s="121" t="s">
-        <v>290</v>
-      </c>
       <c r="V7" s="123" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="W7" s="175">
         <v>40495</v>
@@ -4876,7 +4876,7 @@
         <v>31</v>
       </c>
       <c r="AA7" s="132" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB7" s="138" t="s">
         <v>25</v>
@@ -4900,7 +4900,7 @@
       </c>
       <c r="AL7" s="131"/>
       <c r="AM7" s="139" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AN7" s="139"/>
       <c r="AO7" s="116"/>
@@ -4913,7 +4913,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G8" s="206"/>
       <c r="H8" s="206"/>
@@ -4928,27 +4928,27 @@
       <c r="O8" s="140"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S8" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="T8" s="3" t="s">
         <v>389</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>390</v>
       </c>
       <c r="U8" s="3"/>
       <c r="V8" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W8" s="182"/>
       <c r="X8" s="182"/>
       <c r="Y8" s="192"/>
       <c r="Z8" s="194"/>
       <c r="AA8" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB8" s="3" t="s">
         <v>25</v>
@@ -4974,10 +4974,10 @@
         <v>40</v>
       </c>
       <c r="E9" s="51" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F9" s="158" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G9" s="207" t="s">
         <v>25</v>
@@ -5000,16 +5000,16 @@
         <v>41</v>
       </c>
       <c r="S9" s="51" t="s">
+        <v>353</v>
+      </c>
+      <c r="T9" s="160" t="s">
         <v>354</v>
       </c>
-      <c r="T9" s="160" t="s">
-        <v>355</v>
-      </c>
       <c r="U9" s="159" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="V9" s="51" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="W9" s="183"/>
       <c r="X9" s="183">
@@ -5024,7 +5024,7 @@
         <v>0</v>
       </c>
       <c r="AA9" s="158" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AB9" s="159"/>
       <c r="AG9" s="160"/>
@@ -5044,7 +5044,7 @@
       <c r="AM9" s="160"/>
       <c r="AN9" s="160"/>
       <c r="AO9" s="158" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:41" s="42" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5055,7 +5055,7 @@
         <v>43</v>
       </c>
       <c r="F10" s="75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G10" s="45" t="s">
         <v>25</v>
@@ -5070,7 +5070,7 @@
         <v>44</v>
       </c>
       <c r="M10" s="46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N10" s="47"/>
       <c r="O10" s="110"/>
@@ -5079,16 +5079,16 @@
         <v>29</v>
       </c>
       <c r="R10" s="53" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S10" s="64" t="s">
         <v>45</v>
       </c>
       <c r="T10" s="54" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="U10" s="53" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="V10" s="65">
         <v>39879</v>
@@ -5106,7 +5106,7 @@
         <v>0</v>
       </c>
       <c r="AA10" s="75" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AB10" s="53"/>
       <c r="AG10" s="54"/>
@@ -5124,7 +5124,7 @@
       <c r="AM10" s="54"/>
       <c r="AN10" s="54"/>
       <c r="AO10" s="75" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5135,7 +5135,7 @@
       <c r="D11" s="57"/>
       <c r="E11" s="57"/>
       <c r="F11" s="57" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G11" s="58"/>
       <c r="H11" s="58" t="s">
@@ -5150,10 +5150,10 @@
       <c r="O11" s="58"/>
       <c r="P11" s="57"/>
       <c r="Q11" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R11" s="57" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S11" s="55"/>
       <c r="U11" s="57"/>
@@ -5181,10 +5181,10 @@
         <v>47</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F12" s="75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G12" s="45" t="s">
         <v>25</v>
@@ -5213,13 +5213,13 @@
         <v>48</v>
       </c>
       <c r="S12" s="64" t="s">
+        <v>421</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="U12" s="53" t="s">
         <v>422</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="U12" s="53" t="s">
-        <v>423</v>
       </c>
       <c r="V12" s="163">
         <v>40575</v>
@@ -5229,7 +5229,7 @@
       <c r="Y12" s="218"/>
       <c r="Z12" s="219"/>
       <c r="AA12" s="75" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AB12" s="53" t="s">
         <v>25</v>
@@ -5261,13 +5261,13 @@
     </row>
     <row r="13" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="115" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C13" s="115"/>
       <c r="D13" s="115"/>
       <c r="E13" s="115"/>
       <c r="F13" s="116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G13" s="133"/>
       <c r="H13" s="134"/>
@@ -5285,19 +5285,19 @@
         <v>29</v>
       </c>
       <c r="R13" s="121" t="s">
+        <v>266</v>
+      </c>
+      <c r="S13" s="122" t="s">
         <v>267</v>
       </c>
-      <c r="S13" s="122" t="s">
+      <c r="T13" s="120" t="s">
         <v>268</v>
       </c>
-      <c r="T13" s="120" t="s">
+      <c r="U13" s="121" t="s">
+        <v>358</v>
+      </c>
+      <c r="V13" s="141" t="s">
         <v>269</v>
-      </c>
-      <c r="U13" s="121" t="s">
-        <v>359</v>
-      </c>
-      <c r="V13" s="141" t="s">
-        <v>270</v>
       </c>
       <c r="W13" s="175">
         <v>39252</v>
@@ -5314,7 +5314,7 @@
         <v>72</v>
       </c>
       <c r="AA13" s="116" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB13" s="121"/>
       <c r="AC13" s="115"/>
@@ -5341,11 +5341,11 @@
     </row>
     <row r="14" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="42" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E14" s="44"/>
       <c r="F14" s="77" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G14" s="45"/>
       <c r="H14" s="46"/>
@@ -5363,16 +5363,16 @@
         <v>29</v>
       </c>
       <c r="R14" s="53" t="s">
+        <v>247</v>
+      </c>
+      <c r="S14" s="64" t="s">
         <v>248</v>
       </c>
-      <c r="S14" s="64" t="s">
-        <v>249</v>
-      </c>
       <c r="T14" s="54" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="U14" s="53" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="V14" s="65">
         <v>40205</v>
@@ -5390,7 +5390,7 @@
         <v>0</v>
       </c>
       <c r="AA14" s="77" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AB14" s="48"/>
       <c r="AC14" s="44"/>
@@ -5413,15 +5413,15 @@
     </row>
     <row r="15" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="115" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C15" s="115"/>
       <c r="D15" s="115"/>
       <c r="E15" s="115" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F15" s="116" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G15" s="133" t="s">
         <v>31</v>
@@ -5438,30 +5438,30 @@
         <v>31</v>
       </c>
       <c r="M15" s="134" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N15" s="135"/>
       <c r="O15" s="142" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P15" s="119"/>
       <c r="Q15" s="120" t="s">
         <v>29</v>
       </c>
       <c r="R15" s="121" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S15" s="122" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="T15" s="120" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U15" s="121" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="V15" s="141" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="W15" s="175"/>
       <c r="X15" s="175">
@@ -5476,7 +5476,7 @@
         <v>0</v>
       </c>
       <c r="AA15" s="116" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB15" s="121"/>
       <c r="AC15" s="115"/>
@@ -5511,7 +5511,7 @@
       <c r="D16" s="115"/>
       <c r="E16" s="115"/>
       <c r="F16" s="116" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G16" s="133" t="s">
         <v>25</v>
@@ -5542,16 +5542,16 @@
         <v>50</v>
       </c>
       <c r="S16" s="122" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T16" s="120" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="U16" s="121" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="V16" s="141" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="W16" s="175">
         <v>40360</v>
@@ -5568,7 +5568,7 @@
         <v>36</v>
       </c>
       <c r="AA16" s="116" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB16" s="121"/>
       <c r="AC16" s="115"/>
@@ -5600,10 +5600,10 @@
       <c r="C17" s="131"/>
       <c r="D17" s="131"/>
       <c r="E17" s="131" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F17" s="132" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G17" s="133" t="s">
         <v>25</v>
@@ -5618,7 +5618,7 @@
         <v>25</v>
       </c>
       <c r="M17" s="134" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N17" s="135" t="s">
         <v>25</v>
@@ -5628,22 +5628,22 @@
       </c>
       <c r="P17" s="137"/>
       <c r="Q17" s="120" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R17" s="138" t="s">
         <v>52</v>
       </c>
       <c r="S17" s="122" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="T17" s="139" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U17" s="138" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="V17" s="141" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W17" s="175"/>
       <c r="X17" s="175"/>
@@ -5680,14 +5680,14 @@
     <row r="18" spans="2:41" s="51" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="124"/>
       <c r="C18" s="124" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D18" s="124"/>
       <c r="E18" s="124" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F18" s="125" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G18" s="203"/>
       <c r="H18" s="204"/>
@@ -5706,22 +5706,22 @@
       <c r="O18" s="127"/>
       <c r="P18" s="128"/>
       <c r="Q18" s="129" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R18" s="126" t="s">
+        <v>181</v>
+      </c>
+      <c r="S18" s="124" t="s">
+        <v>194</v>
+      </c>
+      <c r="T18" s="129" t="s">
         <v>182</v>
       </c>
-      <c r="S18" s="124" t="s">
-        <v>195</v>
-      </c>
-      <c r="T18" s="129" t="s">
-        <v>183</v>
-      </c>
       <c r="U18" s="121" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="V18" s="124" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="W18" s="176">
         <v>41383</v>
@@ -5752,7 +5752,7 @@
       </c>
       <c r="AL18" s="124"/>
       <c r="AM18" s="129" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AN18" s="129"/>
       <c r="AO18" s="125"/>
@@ -5764,7 +5764,7 @@
       <c r="D19" s="44"/>
       <c r="E19" s="44"/>
       <c r="F19" s="77" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G19" s="45" t="s">
         <v>25</v>
@@ -5802,11 +5802,11 @@
         <v>34</v>
       </c>
       <c r="T19" s="54" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="U19" s="48"/>
       <c r="V19" s="66" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="W19" s="177">
         <v>40668</v>
@@ -5823,7 +5823,7 @@
         <v>25</v>
       </c>
       <c r="AA19" s="77" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AB19" s="48"/>
       <c r="AC19" s="44"/>
@@ -5842,18 +5842,18 @@
       <c r="AM19" s="49"/>
       <c r="AN19" s="49"/>
       <c r="AO19" s="77" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="20" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" s="42" t="s">
+        <v>467</v>
+      </c>
+      <c r="E20" s="42" t="s">
         <v>468</v>
       </c>
-      <c r="E20" s="42" t="s">
-        <v>469</v>
-      </c>
       <c r="F20" s="75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G20" s="45" t="s">
         <v>25</v>
@@ -5880,7 +5880,7 @@
       <c r="O20" s="110"/>
       <c r="P20" s="103"/>
       <c r="Q20" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R20" s="53" t="s">
         <v>54</v>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="U20" s="53"/>
       <c r="V20" s="66" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="W20" s="177"/>
       <c r="X20" s="177"/>
@@ -5923,7 +5923,7 @@
       <c r="AM20" s="54"/>
       <c r="AN20" s="54"/>
       <c r="AO20" s="75" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="21" spans="2:41" s="51" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -5933,10 +5933,10 @@
       </c>
       <c r="D21" s="124"/>
       <c r="E21" s="124" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F21" s="125" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G21" s="203" t="s">
         <v>25</v>
@@ -5970,13 +5970,13 @@
         <v>59</v>
       </c>
       <c r="T21" s="129" t="s">
+        <v>290</v>
+      </c>
+      <c r="U21" s="121" t="s">
         <v>291</v>
       </c>
-      <c r="U21" s="121" t="s">
-        <v>292</v>
-      </c>
       <c r="V21" s="124" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="W21" s="176"/>
       <c r="X21" s="176">
@@ -5991,7 +5991,7 @@
         <v>0</v>
       </c>
       <c r="AA21" s="125" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB21" s="126" t="s">
         <v>25</v>
@@ -6025,14 +6025,14 @@
     <row r="22" spans="2:41" s="63" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>60</v>
+        <v>539</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F22" s="76" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G22" s="201"/>
       <c r="H22" s="11"/>
@@ -6047,20 +6047,20 @@
       <c r="O22" s="89"/>
       <c r="P22" s="102"/>
       <c r="Q22" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R22" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="S22" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="S22" s="12" t="s">
-        <v>62</v>
       </c>
       <c r="T22" s="33" t="s">
         <v>57</v>
       </c>
       <c r="U22" s="32"/>
       <c r="V22" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="W22" s="178"/>
       <c r="X22" s="178"/>
@@ -6088,12 +6088,12 @@
     </row>
     <row r="23" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="44" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D23" s="44"/>
       <c r="E23" s="44"/>
       <c r="F23" s="77" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G23" s="45" t="s">
         <v>25</v>
@@ -6116,22 +6116,22 @@
       <c r="O23" s="109"/>
       <c r="P23" s="101"/>
       <c r="Q23" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R23" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="S23" s="152" t="s">
+        <v>202</v>
+      </c>
+      <c r="T23" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="S23" s="152" t="s">
-        <v>203</v>
-      </c>
-      <c r="T23" s="49" t="s">
-        <v>64</v>
-      </c>
       <c r="U23" s="48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="V23" s="69" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W23" s="179">
         <v>41085</v>
@@ -6170,12 +6170,12 @@
     </row>
     <row r="24" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D24" s="44"/>
       <c r="E24" s="44"/>
       <c r="F24" s="77" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G24" s="45" t="s">
         <v>25</v>
@@ -6196,7 +6196,7 @@
         <v>25</v>
       </c>
       <c r="M24" s="46" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N24" s="47"/>
       <c r="O24" s="109"/>
@@ -6205,19 +6205,19 @@
         <v>29</v>
       </c>
       <c r="R24" s="53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S24" s="64" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T24" s="49" t="s">
+        <v>394</v>
+      </c>
+      <c r="U24" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="U24" s="2" t="s">
-        <v>396</v>
-      </c>
       <c r="V24" s="69" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="W24" s="179">
         <v>41037</v>
@@ -6234,7 +6234,7 @@
         <v>13</v>
       </c>
       <c r="AA24" s="77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB24" s="48" t="s">
         <v>25</v>
@@ -6261,12 +6261,12 @@
     </row>
     <row r="25" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D25" s="44"/>
       <c r="E25" s="44"/>
       <c r="F25" s="77" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G25" s="45" t="s">
         <v>25</v>
@@ -6283,7 +6283,7 @@
       </c>
       <c r="L25" s="46"/>
       <c r="M25" s="46" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N25" s="47"/>
       <c r="O25" s="109"/>
@@ -6292,17 +6292,17 @@
         <v>29</v>
       </c>
       <c r="R25" s="53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="S25" s="64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T25" s="49" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="U25" s="48"/>
       <c r="V25" s="69" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W25" s="179"/>
       <c r="X25" s="179">
@@ -6317,7 +6317,7 @@
         <v>0</v>
       </c>
       <c r="AA25" s="77" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB25" s="48" t="s">
         <v>25</v>
@@ -6338,23 +6338,23 @@
         <v>25</v>
       </c>
       <c r="AM25" s="49" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AN25" s="49"/>
       <c r="AO25" s="77" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="26" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D26" s="44"/>
       <c r="E26" s="44" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F26" s="43" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G26" s="45" t="s">
         <v>25</v>
@@ -6373,7 +6373,7 @@
         <v>25</v>
       </c>
       <c r="M26" s="46" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N26" s="47"/>
       <c r="O26" s="109"/>
@@ -6382,15 +6382,15 @@
         <v>29</v>
       </c>
       <c r="R26" s="53" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S26" s="64"/>
       <c r="T26" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U26" s="48"/>
       <c r="V26" s="153" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="W26" s="179"/>
       <c r="X26" s="179"/>
@@ -6403,7 +6403,7 @@
         <v>0</v>
       </c>
       <c r="AA26" s="77" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB26" s="48"/>
       <c r="AC26" s="44"/>
@@ -6428,14 +6428,14 @@
     </row>
     <row r="27" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D27" s="44"/>
       <c r="E27" s="44" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F27" s="43" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G27" s="45" t="s">
         <v>25</v>
@@ -6461,17 +6461,17 @@
         <v>29</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="S27" s="64" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="T27" s="49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="U27" s="48"/>
       <c r="V27" s="69" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="W27" s="179">
         <v>41244</v>
@@ -6488,7 +6488,7 @@
         <v>7</v>
       </c>
       <c r="AA27" s="77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB27" s="48" t="s">
         <v>25</v>
@@ -6517,12 +6517,12 @@
     </row>
     <row r="28" spans="2:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="57" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D28" s="57"/>
       <c r="E28" s="57"/>
       <c r="F28" s="169" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G28" s="58"/>
       <c r="H28" s="58"/>
@@ -6537,35 +6537,35 @@
         <v>25</v>
       </c>
       <c r="M28" s="58" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N28" s="58"/>
       <c r="O28" s="170"/>
       <c r="P28" s="57"/>
       <c r="Q28" s="57" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="S28" s="55" t="s">
+        <v>503</v>
+      </c>
+      <c r="T28" s="57" t="s">
+        <v>501</v>
+      </c>
+      <c r="U28" s="174" t="s">
+        <v>505</v>
+      </c>
+      <c r="V28" s="171" t="s">
         <v>504</v>
-      </c>
-      <c r="T28" s="57" t="s">
-        <v>502</v>
-      </c>
-      <c r="U28" s="174" t="s">
-        <v>506</v>
-      </c>
-      <c r="V28" s="171" t="s">
-        <v>505</v>
       </c>
       <c r="W28" s="185"/>
       <c r="X28" s="185"/>
       <c r="Y28" s="192"/>
       <c r="Z28" s="194"/>
       <c r="AA28" s="57" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB28" s="57"/>
       <c r="AC28" s="57"/>
@@ -6587,10 +6587,10 @@
     </row>
     <row r="29" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C29" s="42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F29" s="43" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G29" s="45"/>
       <c r="H29" s="46"/>
@@ -6603,16 +6603,16 @@
       <c r="O29" s="162"/>
       <c r="P29" s="103"/>
       <c r="Q29" s="54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R29" s="53"/>
       <c r="S29" s="64"/>
       <c r="T29" s="54" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="U29" s="53"/>
       <c r="V29" s="66" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="W29" s="177"/>
       <c r="X29" s="177"/>
@@ -6633,10 +6633,10 @@
     </row>
     <row r="30" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F30" s="75" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G30" s="45" t="s">
         <v>25</v>
@@ -6654,19 +6654,19 @@
         <v>29</v>
       </c>
       <c r="R30" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="S30" s="64" t="s">
+        <v>198</v>
+      </c>
+      <c r="T30" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="S30" s="64" t="s">
-        <v>199</v>
-      </c>
-      <c r="T30" s="54" t="s">
-        <v>67</v>
-      </c>
       <c r="U30" s="53" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="V30" s="65" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="W30" s="177">
         <v>40269</v>
@@ -6683,7 +6683,7 @@
         <v>39</v>
       </c>
       <c r="AA30" s="75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB30" s="53" t="s">
         <v>25</v>
@@ -6707,20 +6707,20 @@
       <c r="AM30" s="54"/>
       <c r="AN30" s="54"/>
       <c r="AO30" s="75" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="31" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C31" s="44"/>
       <c r="D31" s="44"/>
       <c r="E31" s="44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F31" s="77" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G31" s="45" t="s">
         <v>25</v>
@@ -6744,17 +6744,17 @@
         <v>29</v>
       </c>
       <c r="R31" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="S31" s="156" t="s">
         <v>152</v>
       </c>
-      <c r="S31" s="156" t="s">
+      <c r="T31" s="49" t="s">
         <v>153</v>
-      </c>
-      <c r="T31" s="49" t="s">
-        <v>154</v>
       </c>
       <c r="U31" s="48"/>
       <c r="V31" s="153" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="W31" s="179">
         <v>40840</v>
@@ -6771,7 +6771,7 @@
         <v>20</v>
       </c>
       <c r="AA31" s="77" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AB31" s="48"/>
       <c r="AC31" s="44"/>
@@ -6793,11 +6793,11 @@
     </row>
     <row r="32" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="154"/>
       <c r="F32" s="75" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G32" s="45"/>
       <c r="H32" s="46"/>
@@ -6812,20 +6812,20 @@
       <c r="O32" s="110"/>
       <c r="P32" s="103"/>
       <c r="Q32" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R32" s="53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S32" s="64"/>
       <c r="T32" s="54" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="V32" s="66" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="W32" s="177">
         <v>40563</v>
@@ -6858,13 +6858,13 @@
     </row>
     <row r="33" spans="2:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="57"/>
       <c r="D33" s="57"/>
       <c r="E33" s="57"/>
       <c r="F33" s="57" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G33" s="58" t="s">
         <v>25</v>
@@ -6885,16 +6885,16 @@
       <c r="O33" s="58"/>
       <c r="P33" s="57"/>
       <c r="Q33" s="57" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R33" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="S33" s="165" t="s">
         <v>71</v>
       </c>
-      <c r="S33" s="165" t="s">
-        <v>72</v>
-      </c>
       <c r="T33" s="57" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="U33" s="57"/>
       <c r="V33" s="166">
@@ -6905,7 +6905,7 @@
       <c r="Y33" s="192"/>
       <c r="Z33" s="194"/>
       <c r="AA33" s="57" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AB33" s="57" t="s">
         <v>25</v>
@@ -6932,18 +6932,18 @@
       <c r="AM33" s="57"/>
       <c r="AN33" s="57"/>
       <c r="AO33" s="57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B34" s="42" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="51"/>
       <c r="E34" s="51"/>
       <c r="F34" s="158" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G34" s="207" t="s">
         <v>25</v>
@@ -6969,17 +6969,17 @@
         <v>29</v>
       </c>
       <c r="R34" s="159" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="S34" s="216" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="T34" s="160" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="U34" s="159"/>
       <c r="V34" s="217" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="W34" s="183"/>
       <c r="X34" s="183">
@@ -6994,7 +6994,7 @@
         <v>0</v>
       </c>
       <c r="AA34" s="158" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB34" s="159" t="s">
         <v>25</v>
@@ -7023,13 +7023,13 @@
     </row>
     <row r="35" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F35" s="75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G35" s="45" t="s">
         <v>25</v>
@@ -7048,15 +7048,15 @@
       <c r="O35" s="110"/>
       <c r="P35" s="103"/>
       <c r="Q35" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R35" s="53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S35" s="64"/>
       <c r="T35" s="54"/>
       <c r="U35" s="53" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="V35" s="163">
         <v>40756</v>
@@ -7074,7 +7074,7 @@
         <v>23</v>
       </c>
       <c r="AA35" s="75" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AB35" s="53"/>
       <c r="AG35" s="54"/>
@@ -7092,18 +7092,18 @@
       <c r="AM35" s="54"/>
       <c r="AN35" s="54"/>
       <c r="AO35" s="75" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="36" spans="2:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="74" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>25</v>
@@ -7121,13 +7121,13 @@
         <v>29</v>
       </c>
       <c r="R36" s="164" t="s">
+        <v>464</v>
+      </c>
+      <c r="S36" s="61" t="s">
         <v>465</v>
       </c>
-      <c r="S36" s="61" t="s">
+      <c r="T36" s="23" t="s">
         <v>466</v>
-      </c>
-      <c r="T36" s="23" t="s">
-        <v>467</v>
       </c>
       <c r="U36" s="22"/>
       <c r="V36" s="62">
@@ -7165,10 +7165,10 @@
     </row>
     <row r="37" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F37" s="75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G37" s="45" t="s">
         <v>25</v>
@@ -7185,22 +7185,22 @@
       <c r="O37" s="110"/>
       <c r="P37" s="103"/>
       <c r="Q37" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="R37" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="S37" s="64" t="s">
+        <v>461</v>
+      </c>
+      <c r="T37" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="R37" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="S37" s="64" t="s">
+      <c r="U37" s="53" t="s">
         <v>462</v>
       </c>
-      <c r="T37" s="54" t="s">
-        <v>79</v>
-      </c>
-      <c r="U37" s="53" t="s">
+      <c r="V37" s="163" t="s">
         <v>463</v>
-      </c>
-      <c r="V37" s="163" t="s">
-        <v>464</v>
       </c>
       <c r="W37" s="177">
         <v>41331</v>
@@ -7215,7 +7215,7 @@
         <v>4</v>
       </c>
       <c r="AA37" s="75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB37" s="53"/>
       <c r="AG37" s="54"/>
@@ -7236,13 +7236,13 @@
     </row>
     <row r="38" spans="2:41" s="63" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="76" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G38" s="201"/>
       <c r="H38" s="11"/>
@@ -7257,18 +7257,18 @@
       <c r="O38" s="89"/>
       <c r="P38" s="102"/>
       <c r="Q38" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R38" s="32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="S38" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="T38" s="33"/>
       <c r="U38" s="34"/>
       <c r="V38" s="143" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="W38" s="178">
         <v>40443</v>
@@ -7293,15 +7293,15 @@
       <c r="AM38" s="33"/>
       <c r="AN38" s="33"/>
       <c r="AO38" s="76" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="39" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="44" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F39" s="75" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G39" s="45"/>
       <c r="H39" s="46"/>
@@ -7316,18 +7316,18 @@
       <c r="O39" s="162"/>
       <c r="P39" s="103"/>
       <c r="Q39" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R39" s="173" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="S39" s="64"/>
       <c r="T39" s="54" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="U39" s="48"/>
       <c r="V39" s="65" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="W39" s="177">
         <v>41061</v>
@@ -7355,13 +7355,13 @@
     </row>
     <row r="40" spans="2:41" s="51" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" s="42"/>
       <c r="D40" s="42"/>
       <c r="E40" s="42"/>
       <c r="F40" s="75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G40" s="45" t="s">
         <v>25</v>
@@ -7387,25 +7387,25 @@
       </c>
       <c r="O40" s="110"/>
       <c r="P40" s="103" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="Q40" s="54" t="s">
         <v>29</v>
       </c>
       <c r="R40" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="S40" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="S40" s="64" t="s">
-        <v>82</v>
-      </c>
       <c r="T40" s="54" t="s">
+        <v>300</v>
+      </c>
+      <c r="U40" s="53" t="s">
         <v>301</v>
       </c>
-      <c r="U40" s="53" t="s">
-        <v>302</v>
-      </c>
       <c r="V40" s="66" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="W40" s="177">
         <v>40544</v>
@@ -7422,7 +7422,7 @@
         <v>30</v>
       </c>
       <c r="AA40" s="75" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB40" s="53" t="s">
         <v>25</v>
@@ -7451,13 +7451,13 @@
     </row>
     <row r="41" spans="2:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="78" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G41" s="18" t="s">
         <v>25</v>
@@ -7484,22 +7484,22 @@
       <c r="O41" s="111"/>
       <c r="P41" s="104"/>
       <c r="Q41" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R41" s="96" t="s">
+        <v>83</v>
+      </c>
+      <c r="S41" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="S41" s="68" t="s">
-        <v>85</v>
-      </c>
       <c r="T41" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U41" s="172" t="s">
+        <v>411</v>
+      </c>
+      <c r="V41" s="67" t="s">
         <v>412</v>
-      </c>
-      <c r="V41" s="67" t="s">
-        <v>413</v>
       </c>
       <c r="W41" s="186">
         <v>40878</v>
@@ -7542,18 +7542,18 @@
       <c r="AM41" s="31"/>
       <c r="AN41" s="31"/>
       <c r="AO41" s="74" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="42" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="42" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E42" s="44" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F42" s="77" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G42" s="45" t="s">
         <v>31</v>
@@ -7564,7 +7564,7 @@
       <c r="K42" s="46"/>
       <c r="L42" s="46"/>
       <c r="M42" s="46" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N42" s="47"/>
       <c r="O42" s="88"/>
@@ -7573,19 +7573,19 @@
         <v>29</v>
       </c>
       <c r="R42" s="53" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="S42" s="64" t="s">
+        <v>408</v>
+      </c>
+      <c r="T42" s="54" t="s">
+        <v>406</v>
+      </c>
+      <c r="U42" s="53" t="s">
         <v>409</v>
       </c>
-      <c r="T42" s="54" t="s">
-        <v>407</v>
-      </c>
-      <c r="U42" s="53" t="s">
+      <c r="V42" s="65" t="s">
         <v>410</v>
-      </c>
-      <c r="V42" s="65" t="s">
-        <v>411</v>
       </c>
       <c r="W42" s="177"/>
       <c r="X42" s="177">
@@ -7600,7 +7600,7 @@
         <v>0</v>
       </c>
       <c r="AA42" s="77" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB42" s="48" t="s">
         <v>25</v>
@@ -7622,13 +7622,13 @@
     </row>
     <row r="43" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="115" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C43" s="115"/>
       <c r="D43" s="115"/>
       <c r="E43" s="115"/>
       <c r="F43" s="116" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G43" s="133"/>
       <c r="H43" s="134"/>
@@ -7652,19 +7652,19 @@
         <v>29</v>
       </c>
       <c r="R43" s="121" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S43" s="122" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="T43" s="120" t="s">
+        <v>361</v>
+      </c>
+      <c r="U43" s="121" t="s">
         <v>362</v>
       </c>
-      <c r="U43" s="121" t="s">
-        <v>363</v>
-      </c>
       <c r="V43" s="144" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="W43" s="175"/>
       <c r="X43" s="175">
@@ -7679,7 +7679,7 @@
         <v>0</v>
       </c>
       <c r="AA43" s="116" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB43" s="121" t="s">
         <v>25</v>
@@ -7713,18 +7713,18 @@
       </c>
       <c r="AN43" s="120"/>
       <c r="AO43" s="116" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="44" spans="2:41" s="63" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="76" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G44" s="201"/>
       <c r="H44" s="11"/>
@@ -7738,21 +7738,21 @@
       <c r="N44" s="202"/>
       <c r="O44" s="89"/>
       <c r="P44" s="102" t="s">
+        <v>321</v>
+      </c>
+      <c r="Q44" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="R44" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="S44" s="12" t="s">
         <v>322</v>
-      </c>
-      <c r="Q44" s="33" t="s">
-        <v>216</v>
-      </c>
-      <c r="R44" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="S44" s="12" t="s">
-        <v>323</v>
       </c>
       <c r="T44" s="33"/>
       <c r="U44" s="24"/>
       <c r="V44" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="W44" s="178"/>
       <c r="X44" s="178"/>
@@ -7780,13 +7780,13 @@
     </row>
     <row r="45" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E45" s="42" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F45" s="75" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G45" s="45"/>
       <c r="H45" s="46"/>
@@ -7795,7 +7795,7 @@
       <c r="K45" s="46"/>
       <c r="L45" s="46"/>
       <c r="M45" s="46" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="N45" s="47"/>
       <c r="O45" s="110"/>
@@ -7804,17 +7804,17 @@
         <v>29</v>
       </c>
       <c r="R45" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="S45" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="S45" s="64" t="s">
+      <c r="T45" s="54" t="s">
         <v>92</v>
-      </c>
-      <c r="T45" s="54" t="s">
-        <v>93</v>
       </c>
       <c r="U45" s="52"/>
       <c r="V45" s="66" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="W45" s="177"/>
       <c r="X45" s="177">
@@ -7829,7 +7829,7 @@
         <v>0</v>
       </c>
       <c r="AA45" s="75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB45" s="53"/>
       <c r="AG45" s="54"/>
@@ -7846,13 +7846,13 @@
     </row>
     <row r="46" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="115" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C46" s="115"/>
       <c r="D46" s="115"/>
       <c r="E46" s="115"/>
       <c r="F46" s="116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G46" s="133"/>
       <c r="H46" s="134"/>
@@ -7870,19 +7870,19 @@
         <v>29</v>
       </c>
       <c r="R46" s="121" t="s">
+        <v>234</v>
+      </c>
+      <c r="S46" s="122" t="s">
         <v>235</v>
       </c>
-      <c r="S46" s="122" t="s">
+      <c r="T46" s="120" t="s">
+        <v>237</v>
+      </c>
+      <c r="U46" s="121" t="s">
+        <v>329</v>
+      </c>
+      <c r="V46" s="123" t="s">
         <v>236</v>
-      </c>
-      <c r="T46" s="120" t="s">
-        <v>238</v>
-      </c>
-      <c r="U46" s="121" t="s">
-        <v>330</v>
-      </c>
-      <c r="V46" s="123" t="s">
-        <v>237</v>
       </c>
       <c r="W46" s="175">
         <v>41143</v>
@@ -7899,7 +7899,7 @@
         <v>10</v>
       </c>
       <c r="AA46" s="132" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB46" s="138"/>
       <c r="AC46" s="131"/>
@@ -7926,13 +7926,13 @@
     </row>
     <row r="47" spans="2:41" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B47" s="115" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" s="115"/>
       <c r="D47" s="115"/>
       <c r="E47" s="115"/>
       <c r="F47" s="116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G47" s="133"/>
       <c r="H47" s="134"/>
@@ -7950,19 +7950,19 @@
         <v>29</v>
       </c>
       <c r="R47" s="121" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S47" s="122" t="s">
+        <v>331</v>
+      </c>
+      <c r="T47" s="120" t="s">
+        <v>330</v>
+      </c>
+      <c r="U47" s="121" t="s">
         <v>332</v>
       </c>
-      <c r="T47" s="120" t="s">
-        <v>331</v>
-      </c>
-      <c r="U47" s="121" t="s">
-        <v>333</v>
-      </c>
       <c r="V47" s="141" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="W47" s="175">
         <v>40546</v>
@@ -7979,7 +7979,7 @@
         <v>29</v>
       </c>
       <c r="AA47" s="116" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB47" s="121" t="s">
         <v>25</v>
@@ -7999,20 +7999,20 @@
       </c>
       <c r="AL47" s="115"/>
       <c r="AM47" s="120" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AN47" s="120"/>
       <c r="AO47" s="116"/>
     </row>
     <row r="48" spans="2:41" s="51" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="124" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C48" s="124"/>
       <c r="D48" s="124"/>
       <c r="E48" s="124"/>
       <c r="F48" s="125" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G48" s="203" t="s">
         <v>25</v>
@@ -8027,7 +8027,7 @@
       <c r="K48" s="204"/>
       <c r="L48" s="204"/>
       <c r="M48" s="204" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N48" s="205"/>
       <c r="O48" s="127"/>
@@ -8036,19 +8036,19 @@
         <v>29</v>
       </c>
       <c r="R48" s="149" t="s">
+        <v>95</v>
+      </c>
+      <c r="S48" s="124" t="s">
+        <v>199</v>
+      </c>
+      <c r="T48" s="129" t="s">
         <v>96</v>
       </c>
-      <c r="S48" s="124" t="s">
-        <v>200</v>
-      </c>
-      <c r="T48" s="129" t="s">
-        <v>97</v>
-      </c>
       <c r="U48" s="121" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="V48" s="124" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="W48" s="176">
         <v>39545</v>
@@ -8065,7 +8065,7 @@
         <v>62</v>
       </c>
       <c r="AA48" s="125" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB48" s="126" t="s">
         <v>25</v>
@@ -8089,22 +8089,22 @@
       </c>
       <c r="AL48" s="124"/>
       <c r="AM48" s="129" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AN48" s="129" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AO48" s="125"/>
     </row>
     <row r="49" spans="2:41" s="51" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="124" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C49" s="124"/>
       <c r="D49" s="124"/>
       <c r="E49" s="124"/>
       <c r="F49" s="125" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G49" s="203" t="s">
         <v>25</v>
@@ -8123,7 +8123,7 @@
         <v>25</v>
       </c>
       <c r="M49" s="204" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N49" s="205" t="s">
         <v>25</v>
@@ -8136,19 +8136,19 @@
         <v>29</v>
       </c>
       <c r="R49" s="149" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S49" s="124" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T49" s="129" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="U49" s="126" t="s">
+        <v>191</v>
+      </c>
+      <c r="V49" s="124" t="s">
         <v>192</v>
-      </c>
-      <c r="V49" s="124" t="s">
-        <v>193</v>
       </c>
       <c r="W49" s="176">
         <v>39385</v>
@@ -8165,7 +8165,7 @@
         <v>68</v>
       </c>
       <c r="AA49" s="150" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB49" s="126" t="s">
         <v>25</v>
@@ -8196,15 +8196,15 @@
     </row>
     <row r="50" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C50" s="44"/>
       <c r="D50" s="44"/>
       <c r="E50" s="44" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F50" s="77" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G50" s="45"/>
       <c r="H50" s="46" t="s">
@@ -8219,22 +8219,22 @@
       <c r="O50" s="109"/>
       <c r="P50" s="101"/>
       <c r="Q50" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R50" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="S50" s="156" t="s">
         <v>101</v>
       </c>
-      <c r="S50" s="156" t="s">
-        <v>102</v>
-      </c>
       <c r="T50" s="49" t="s">
+        <v>429</v>
+      </c>
+      <c r="U50" s="45" t="s">
         <v>430</v>
       </c>
-      <c r="U50" s="45" t="s">
-        <v>431</v>
-      </c>
       <c r="V50" s="157" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="W50" s="179">
         <v>40865</v>
@@ -8251,7 +8251,7 @@
         <v>19</v>
       </c>
       <c r="AA50" s="77" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AB50" s="48" t="s">
         <v>25</v>
@@ -8270,15 +8270,15 @@
       <c r="AM50" s="49"/>
       <c r="AN50" s="49"/>
       <c r="AO50" s="75" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="51" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F51" s="75" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G51" s="45" t="s">
         <v>25</v>
@@ -8298,19 +8298,19 @@
         <v>29</v>
       </c>
       <c r="R51" s="53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="S51" s="64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="T51" s="54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U51" s="52" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="V51" s="66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="W51" s="177">
         <v>40742</v>
@@ -8327,7 +8327,7 @@
         <v>23</v>
       </c>
       <c r="AA51" s="75" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="AB51" s="53" t="s">
         <v>25</v>
@@ -8355,26 +8355,26 @@
         <v>25</v>
       </c>
       <c r="AM51" s="54" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AN51" s="54"/>
       <c r="AO51" s="75" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="44" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D52" s="44"/>
       <c r="E52" s="44" t="s">
+        <v>437</v>
+      </c>
+      <c r="F52" s="77" t="s">
         <v>438</v>
-      </c>
-      <c r="F52" s="77" t="s">
-        <v>439</v>
       </c>
       <c r="G52" s="45" t="s">
         <v>25</v>
@@ -8392,15 +8392,15 @@
         <v>29</v>
       </c>
       <c r="R52" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="S52" s="64"/>
       <c r="T52" s="54" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="U52" s="53"/>
       <c r="V52" s="66" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="W52" s="177">
         <v>39249</v>
@@ -8417,7 +8417,7 @@
         <v>72</v>
       </c>
       <c r="AA52" s="77" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB52" s="53" t="s">
         <v>25</v>
@@ -8436,18 +8436,18 @@
       <c r="AM52" s="54"/>
       <c r="AN52" s="54"/>
       <c r="AO52" s="75" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="53" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C53" s="44"/>
       <c r="D53" s="44"/>
       <c r="E53" s="44"/>
       <c r="F53" s="77" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G53" s="45" t="s">
         <v>25</v>
@@ -8465,16 +8465,16 @@
         <v>29</v>
       </c>
       <c r="R53" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S53" s="64" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T53" s="54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U53" s="53" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="V53" s="66">
         <v>2005</v>
@@ -8505,18 +8505,18 @@
       <c r="AM53" s="54"/>
       <c r="AN53" s="54"/>
       <c r="AO53" s="75" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="54" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="131" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C54" s="131"/>
       <c r="D54" s="131"/>
       <c r="E54" s="131"/>
       <c r="F54" s="132" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G54" s="133" t="s">
         <v>25</v>
@@ -8546,15 +8546,15 @@
         <v>29</v>
       </c>
       <c r="R54" s="138" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S54" s="122"/>
       <c r="T54" s="139" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U54" s="121"/>
       <c r="V54" s="146" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="W54" s="187">
         <v>39748</v>
@@ -8571,7 +8571,7 @@
         <v>56</v>
       </c>
       <c r="AA54" s="132" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB54" s="121" t="s">
         <v>25</v>
@@ -8599,20 +8599,20 @@
       </c>
       <c r="AL54" s="115"/>
       <c r="AM54" s="120" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AN54" s="120"/>
       <c r="AO54" s="116"/>
     </row>
     <row r="55" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C55" s="44"/>
       <c r="D55" s="44"/>
       <c r="E55" s="44"/>
       <c r="F55" s="77" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G55" s="45"/>
       <c r="H55" s="46" t="s">
@@ -8627,20 +8627,20 @@
       <c r="O55" s="155"/>
       <c r="P55" s="101"/>
       <c r="Q55" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R55" s="48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S55" s="64" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T55" s="54" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="U55" s="45"/>
       <c r="V55" s="66" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="W55" s="177"/>
       <c r="X55" s="177"/>
@@ -8669,13 +8669,13 @@
     </row>
     <row r="56" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="E56" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="E56" s="42" t="s">
-        <v>112</v>
-      </c>
       <c r="F56" s="75" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G56" s="45" t="s">
         <v>25</v>
@@ -8690,14 +8690,14 @@
       <c r="O56" s="110"/>
       <c r="P56" s="103"/>
       <c r="Q56" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R56" s="53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S56" s="64"/>
       <c r="T56" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U56" s="52"/>
       <c r="V56" s="163">
@@ -8716,7 +8716,7 @@
         <v>22</v>
       </c>
       <c r="AA56" s="75" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AB56" s="53"/>
       <c r="AG56" s="54"/>
@@ -8734,18 +8734,18 @@
       <c r="AM56" s="54"/>
       <c r="AN56" s="54"/>
       <c r="AO56" s="75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="2:41" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B57" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E57" s="42" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F57" s="75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G57" s="45"/>
       <c r="H57" s="46"/>
@@ -8760,30 +8760,30 @@
         <v>25</v>
       </c>
       <c r="M57" s="46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N57" s="47"/>
       <c r="O57" s="110"/>
       <c r="P57" s="103" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Q57" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R57" s="173" t="s">
+        <v>448</v>
+      </c>
+      <c r="S57" s="64" t="s">
+        <v>450</v>
+      </c>
+      <c r="T57" s="54" t="s">
         <v>449</v>
       </c>
-      <c r="S57" s="64" t="s">
+      <c r="U57" s="53" t="s">
         <v>451</v>
       </c>
-      <c r="T57" s="54" t="s">
-        <v>450</v>
-      </c>
-      <c r="U57" s="53" t="s">
-        <v>452</v>
-      </c>
       <c r="V57" s="65" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W57" s="177">
         <v>41080</v>
@@ -8798,7 +8798,7 @@
         <v>12</v>
       </c>
       <c r="AA57" s="75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB57" s="53" t="s">
         <v>25</v>
@@ -8828,13 +8828,13 @@
     </row>
     <row r="58" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="115" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C58" s="115"/>
       <c r="D58" s="115"/>
       <c r="E58" s="115"/>
       <c r="F58" s="116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G58" s="133"/>
       <c r="H58" s="134"/>
@@ -8854,19 +8854,19 @@
         <v>29</v>
       </c>
       <c r="R58" s="148" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S58" s="122" t="s">
+        <v>304</v>
+      </c>
+      <c r="T58" s="54" t="s">
         <v>305</v>
       </c>
-      <c r="T58" s="54" t="s">
+      <c r="U58" s="53" t="s">
         <v>306</v>
       </c>
-      <c r="U58" s="53" t="s">
-        <v>307</v>
-      </c>
       <c r="V58" s="144" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W58" s="175">
         <v>41099</v>
@@ -8883,7 +8883,7 @@
         <v>11</v>
       </c>
       <c r="AA58" s="116" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB58" s="121" t="s">
         <v>25</v>
@@ -8905,20 +8905,20 @@
       </c>
       <c r="AL58" s="115"/>
       <c r="AM58" s="120" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AN58" s="120"/>
       <c r="AO58" s="116"/>
     </row>
     <row r="59" spans="2:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G59" s="58"/>
       <c r="H59" s="58"/>
@@ -8932,17 +8932,17 @@
       <c r="N59" s="58"/>
       <c r="O59" s="168"/>
       <c r="Q59" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R59" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="S59" s="55"/>
       <c r="T59" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="V59" s="56" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="W59" s="184"/>
       <c r="X59" s="184"/>
@@ -8951,15 +8951,15 @@
     </row>
     <row r="60" spans="2:41" s="63" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F60" s="76" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G60" s="201"/>
       <c r="H60" s="11"/>
@@ -8974,18 +8974,18 @@
       <c r="O60" s="89"/>
       <c r="P60" s="102"/>
       <c r="Q60" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R60" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S60" s="12"/>
       <c r="T60" s="33" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="U60" s="32"/>
       <c r="V60" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="W60" s="178"/>
       <c r="X60" s="178"/>
@@ -9012,18 +9012,18 @@
       <c r="AM60" s="33"/>
       <c r="AN60" s="33"/>
       <c r="AO60" s="76" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="61" spans="2:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G61" s="58"/>
       <c r="H61" s="58"/>
@@ -9037,18 +9037,18 @@
       <c r="N61" s="58"/>
       <c r="O61" s="168"/>
       <c r="Q61" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R61" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S61" s="55"/>
       <c r="T61" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U61" s="167"/>
       <c r="V61" s="56" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="W61" s="184"/>
       <c r="X61" s="184"/>
@@ -9057,10 +9057,10 @@
     </row>
     <row r="62" spans="2:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G62" s="58"/>
       <c r="H62" s="58"/>
@@ -9074,16 +9074,16 @@
       <c r="N62" s="58"/>
       <c r="O62" s="168"/>
       <c r="Q62" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R62" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S62" s="55" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="V62" s="56" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="W62" s="184"/>
       <c r="X62" s="184"/>
@@ -9092,17 +9092,17 @@
     </row>
     <row r="63" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B63" s="115" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C63" s="115" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D63" s="115"/>
       <c r="E63" s="115" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F63" s="116" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G63" s="133" t="s">
         <v>25</v>
@@ -9132,17 +9132,17 @@
         <v>29</v>
       </c>
       <c r="R63" s="148" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="S63" s="122" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="T63" s="120" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U63" s="121"/>
       <c r="V63" s="144" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="W63" s="175">
         <v>40667</v>
@@ -9159,7 +9159,7 @@
         <v>25</v>
       </c>
       <c r="AA63" s="116" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AB63" s="121" t="s">
         <v>25</v>
@@ -9185,18 +9185,18 @@
       <c r="AM63" s="120"/>
       <c r="AN63" s="120"/>
       <c r="AO63" s="116" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="64" spans="2:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
       <c r="F64" s="74" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G64" s="18" t="s">
         <v>25</v>
@@ -9214,13 +9214,13 @@
         <v>29</v>
       </c>
       <c r="R64" s="95" t="s">
+        <v>127</v>
+      </c>
+      <c r="S64" s="61" t="s">
         <v>128</v>
       </c>
-      <c r="S64" s="61" t="s">
-        <v>129</v>
-      </c>
       <c r="T64" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U64" s="22"/>
       <c r="V64" s="62"/>
@@ -9235,7 +9235,7 @@
         <v>0</v>
       </c>
       <c r="AA64" s="74" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AB64" s="22"/>
       <c r="AC64" s="10"/>
@@ -9258,13 +9258,13 @@
     </row>
     <row r="65" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
       <c r="F65" s="74" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G65" s="18" t="s">
         <v>31</v>
@@ -9282,16 +9282,16 @@
         <v>29</v>
       </c>
       <c r="R65" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="S65" s="151" t="s">
         <v>259</v>
       </c>
-      <c r="S65" s="151" t="s">
+      <c r="T65" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="T65" s="25" t="s">
-        <v>261</v>
-      </c>
       <c r="U65" s="22" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="V65" s="62"/>
       <c r="W65" s="181"/>
@@ -9327,15 +9327,15 @@
     <row r="66" spans="1:41" s="63" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="70"/>
       <c r="B66" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F66" s="76" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G66" s="201"/>
       <c r="H66" s="11"/>
@@ -9353,17 +9353,17 @@
         <v>29</v>
       </c>
       <c r="R66" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S66" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="T66" s="33" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="U66" s="32"/>
       <c r="V66" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="W66" s="178">
         <v>40609</v>
@@ -9374,7 +9374,7 @@
       <c r="Y66" s="192"/>
       <c r="Z66" s="194"/>
       <c r="AA66" s="76" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB66" s="32" t="s">
         <v>25</v>
@@ -9397,15 +9397,15 @@
     </row>
     <row r="67" spans="1:41" s="42" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="115" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C67" s="115"/>
       <c r="D67" s="115"/>
       <c r="E67" s="115" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F67" s="116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G67" s="133"/>
       <c r="H67" s="134"/>
@@ -9423,17 +9423,17 @@
         <v>29</v>
       </c>
       <c r="R67" s="121" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S67" s="122" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="T67" s="120" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="U67" s="121"/>
       <c r="V67" s="141" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="W67" s="175">
         <v>40664</v>
@@ -9450,7 +9450,7 @@
         <v>26</v>
       </c>
       <c r="AA67" s="116" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AB67" s="121" t="s">
         <v>25</v>
@@ -9472,22 +9472,22 @@
       </c>
       <c r="AL67" s="115"/>
       <c r="AM67" s="120" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AN67" s="120"/>
       <c r="AO67" s="116" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="68" spans="1:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G68" s="58"/>
       <c r="H68" s="58"/>
@@ -9501,16 +9501,16 @@
       <c r="N68" s="58"/>
       <c r="O68" s="168"/>
       <c r="Q68" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R68" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S68" s="55" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="V68" s="56" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="W68" s="184"/>
       <c r="X68" s="184"/>
@@ -9522,13 +9522,13 @@
     </row>
     <row r="69" spans="1:41" s="51" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B69" s="124" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C69" s="124"/>
       <c r="D69" s="124"/>
       <c r="E69" s="124"/>
       <c r="F69" s="125" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G69" s="203"/>
       <c r="H69" s="204"/>
@@ -9543,20 +9543,20 @@
       <c r="O69" s="127"/>
       <c r="P69" s="128"/>
       <c r="Q69" s="129" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R69" s="126" t="s">
+        <v>239</v>
+      </c>
+      <c r="S69" s="124" t="s">
         <v>240</v>
       </c>
-      <c r="S69" s="124" t="s">
-        <v>241</v>
-      </c>
       <c r="T69" s="129" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U69" s="126"/>
       <c r="V69" s="124" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W69" s="176">
         <v>40834</v>
@@ -9596,15 +9596,15 @@
     </row>
     <row r="70" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="115" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C70" s="115"/>
       <c r="D70" s="115"/>
       <c r="E70" s="115" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F70" s="116" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G70" s="133"/>
       <c r="H70" s="134"/>
@@ -9621,7 +9621,7 @@
         <v>25</v>
       </c>
       <c r="M70" s="134" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N70" s="135" t="s">
         <v>25</v>
@@ -9631,22 +9631,22 @@
       </c>
       <c r="P70" s="119"/>
       <c r="Q70" s="120" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R70" s="121" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S70" s="122" t="s">
+        <v>373</v>
+      </c>
+      <c r="T70" s="120" t="s">
+        <v>232</v>
+      </c>
+      <c r="U70" s="121" t="s">
+        <v>375</v>
+      </c>
+      <c r="V70" s="123" t="s">
         <v>374</v>
-      </c>
-      <c r="T70" s="120" t="s">
-        <v>233</v>
-      </c>
-      <c r="U70" s="121" t="s">
-        <v>376</v>
-      </c>
-      <c r="V70" s="123" t="s">
-        <v>375</v>
       </c>
       <c r="W70" s="175"/>
       <c r="X70" s="175"/>
@@ -9659,7 +9659,7 @@
         <v>0</v>
       </c>
       <c r="AA70" s="132" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB70" s="138" t="s">
         <v>25</v>
@@ -9684,10 +9684,10 @@
     </row>
     <row r="71" spans="1:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G71" s="58"/>
       <c r="H71" s="58"/>
@@ -9701,13 +9701,13 @@
       <c r="N71" s="58"/>
       <c r="O71" s="167"/>
       <c r="Q71" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R71" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="S71" s="55" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V71" s="56"/>
       <c r="W71" s="184"/>
@@ -9723,13 +9723,13 @@
     </row>
     <row r="72" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B72" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E72" s="42" t="s">
         <v>44</v>
       </c>
       <c r="F72" s="75" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G72" s="45"/>
       <c r="H72" s="46"/>
@@ -9744,20 +9744,20 @@
       <c r="O72" s="110"/>
       <c r="P72" s="103"/>
       <c r="Q72" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R72" s="53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S72" s="64" t="s">
+        <v>413</v>
+      </c>
+      <c r="T72" s="54" t="s">
         <v>414</v>
-      </c>
-      <c r="T72" s="54" t="s">
-        <v>415</v>
       </c>
       <c r="U72" s="53"/>
       <c r="V72" s="66" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="W72" s="177">
         <v>40561</v>
@@ -9793,11 +9793,11 @@
     </row>
     <row r="73" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E73" s="44"/>
       <c r="F73" s="77" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G73" s="45"/>
       <c r="H73" s="46"/>
@@ -9812,16 +9812,16 @@
       <c r="O73" s="88"/>
       <c r="P73" s="101"/>
       <c r="Q73" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R73" s="53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S73" s="64" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="T73" s="54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U73" s="53"/>
       <c r="V73" s="163">
@@ -9840,7 +9840,7 @@
         <v>28</v>
       </c>
       <c r="AA73" s="77" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB73" s="48"/>
       <c r="AC73" s="44"/>
@@ -9867,15 +9867,15 @@
     </row>
     <row r="74" spans="1:41" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
       <c r="E74" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F74" s="74" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G74" s="18" t="s">
         <v>25</v>
@@ -9893,19 +9893,19 @@
         <v>29</v>
       </c>
       <c r="R74" s="95" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S74" s="61" t="s">
+        <v>509</v>
+      </c>
+      <c r="T74" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="U74" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="T74" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="U74" s="22" t="s">
+      <c r="V74" s="62" t="s">
         <v>511</v>
-      </c>
-      <c r="V74" s="62" t="s">
-        <v>512</v>
       </c>
       <c r="W74" s="181">
         <v>40940</v>
@@ -9922,7 +9922,7 @@
         <v>17</v>
       </c>
       <c r="AA74" s="74" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB74" s="22"/>
       <c r="AC74" s="10"/>
@@ -9945,10 +9945,10 @@
     </row>
     <row r="75" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="42" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F75" s="75" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G75" s="45" t="s">
         <v>25</v>
@@ -9968,15 +9968,15 @@
         <v>29</v>
       </c>
       <c r="R75" s="53" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="S75" s="64"/>
       <c r="T75" s="54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="U75" s="53"/>
       <c r="V75" s="65" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="W75" s="177">
         <v>40828</v>
@@ -9993,7 +9993,7 @@
         <v>20</v>
       </c>
       <c r="AA75" s="75" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB75" s="53" t="s">
         <v>25</v>
@@ -10024,13 +10024,13 @@
     </row>
     <row r="76" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="42" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E76" s="44" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F76" s="77" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G76" s="45"/>
       <c r="H76" s="46" t="s">
@@ -10045,20 +10045,20 @@
       <c r="O76" s="109"/>
       <c r="P76" s="101"/>
       <c r="Q76" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R76" s="53" t="s">
+        <v>253</v>
+      </c>
+      <c r="S76" s="64" t="s">
         <v>254</v>
       </c>
-      <c r="S76" s="64" t="s">
-        <v>255</v>
-      </c>
       <c r="T76" s="54" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="U76" s="53"/>
       <c r="V76" s="66" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="W76" s="177">
         <v>41410</v>
@@ -10091,10 +10091,10 @@
     </row>
     <row r="77" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F77" s="75" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G77" s="45"/>
       <c r="H77" s="46"/>
@@ -10114,13 +10114,13 @@
         <v>29</v>
       </c>
       <c r="R77" s="53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S77" s="64" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="T77" s="54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U77" s="53"/>
       <c r="V77" s="163">
@@ -10139,7 +10139,7 @@
         <v>0</v>
       </c>
       <c r="AA77" s="75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB77" s="53" t="s">
         <v>25</v>
@@ -10158,18 +10158,18 @@
       <c r="AM77" s="54"/>
       <c r="AN77" s="54"/>
       <c r="AO77" s="75" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="78" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E78" s="42" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F78" s="75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G78" s="45" t="s">
         <v>25</v>
@@ -10193,17 +10193,17 @@
         <v>29</v>
       </c>
       <c r="R78" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="S78" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="S78" s="64" t="s">
-        <v>145</v>
-      </c>
       <c r="T78" s="54" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="U78" s="53"/>
       <c r="V78" s="65" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="W78" s="177">
         <v>40252</v>
@@ -10218,7 +10218,7 @@
         <v>39</v>
       </c>
       <c r="AA78" s="75" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AB78" s="53" t="s">
         <v>25</v>
@@ -10248,18 +10248,18 @@
       <c r="AM78" s="54"/>
       <c r="AN78" s="54"/>
       <c r="AO78" s="75" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="79" spans="1:41" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G79" s="58" t="s">
         <v>25</v>
@@ -10273,7 +10273,7 @@
       <c r="N79" s="58"/>
       <c r="O79" s="167"/>
       <c r="Q79" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S79" s="55"/>
       <c r="V79" s="56">
@@ -10303,13 +10303,13 @@
     </row>
     <row r="80" spans="1:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B80" s="131" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C80" s="131"/>
       <c r="D80" s="131"/>
       <c r="E80" s="131"/>
       <c r="F80" s="132" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G80" s="133"/>
       <c r="H80" s="134"/>
@@ -10328,16 +10328,16 @@
       </c>
       <c r="P80" s="137"/>
       <c r="Q80" s="120" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R80" s="121" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="S80" s="122" t="s">
+        <v>228</v>
+      </c>
+      <c r="T80" s="120" t="s">
         <v>229</v>
-      </c>
-      <c r="T80" s="120" t="s">
-        <v>230</v>
       </c>
       <c r="U80" s="138"/>
       <c r="V80" s="141"/>
@@ -10373,15 +10373,15 @@
     </row>
     <row r="81" spans="2:41" s="63" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F81" s="76" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G81" s="201" t="s">
         <v>25</v>
@@ -10398,10 +10398,10 @@
       <c r="O81" s="89"/>
       <c r="P81" s="102"/>
       <c r="Q81" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R81" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S81" s="12"/>
       <c r="T81" s="33"/>
@@ -10438,15 +10438,15 @@
       <c r="AM81" s="33"/>
       <c r="AN81" s="33"/>
       <c r="AO81" s="76" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="82" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F82" s="75" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G82" s="45" t="s">
         <v>25</v>
@@ -10460,17 +10460,17 @@
       <c r="N82" s="47"/>
       <c r="O82" s="110"/>
       <c r="P82" s="103" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="Q82" s="54" t="s">
         <v>29</v>
       </c>
       <c r="R82" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S82" s="64"/>
       <c r="T82" s="54" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="U82" s="53"/>
       <c r="V82" s="66"/>
@@ -10485,7 +10485,7 @@
         <v>0</v>
       </c>
       <c r="AA82" s="77" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AB82" s="48"/>
       <c r="AC82" s="44"/>
@@ -10507,10 +10507,10 @@
     </row>
     <row r="83" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F83" s="75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G83" s="45" t="s">
         <v>25</v>
@@ -10527,7 +10527,7 @@
       </c>
       <c r="L83" s="46"/>
       <c r="M83" s="46" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N83" s="47"/>
       <c r="O83" s="110"/>
@@ -10536,11 +10536,11 @@
         <v>29</v>
       </c>
       <c r="R83" s="53" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S83" s="64"/>
       <c r="T83" s="54" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="U83" s="53"/>
       <c r="V83" s="66"/>
@@ -10555,7 +10555,7 @@
         <v>0</v>
       </c>
       <c r="AA83" s="75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB83" s="53" t="s">
         <v>25</v>
@@ -10572,10 +10572,10 @@
     </row>
     <row r="84" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="42" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F84" s="75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G84" s="45"/>
       <c r="H84" s="46"/>
@@ -10599,19 +10599,19 @@
         <v>29</v>
       </c>
       <c r="R84" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="S84" s="64" t="s">
+        <v>485</v>
+      </c>
+      <c r="T84" s="54" t="s">
         <v>272</v>
       </c>
-      <c r="S84" s="64" t="s">
+      <c r="U84" s="53" t="s">
+        <v>483</v>
+      </c>
+      <c r="V84" s="66" t="s">
         <v>486</v>
-      </c>
-      <c r="T84" s="54" t="s">
-        <v>273</v>
-      </c>
-      <c r="U84" s="53" t="s">
-        <v>484</v>
-      </c>
-      <c r="V84" s="66" t="s">
-        <v>487</v>
       </c>
       <c r="W84" s="177">
         <v>39794</v>
@@ -10628,7 +10628,7 @@
         <v>54</v>
       </c>
       <c r="AA84" s="75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB84" s="53" t="s">
         <v>25</v>
@@ -10642,15 +10642,15 @@
       <c r="AM84" s="54"/>
       <c r="AN84" s="54"/>
       <c r="AO84" s="75" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="85" spans="2:41" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="42" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F85" s="75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G85" s="45"/>
       <c r="H85" s="46"/>
@@ -10667,22 +10667,22 @@
       <c r="O85" s="110"/>
       <c r="P85" s="103"/>
       <c r="Q85" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R85" s="53" t="s">
+        <v>477</v>
+      </c>
+      <c r="S85" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="T85" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="U85" s="53" t="s">
+        <v>476</v>
+      </c>
+      <c r="V85" s="163" t="s">
         <v>478</v>
-      </c>
-      <c r="S85" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="T85" s="54" t="s">
-        <v>148</v>
-      </c>
-      <c r="U85" s="53" t="s">
-        <v>477</v>
-      </c>
-      <c r="V85" s="163" t="s">
-        <v>479</v>
       </c>
       <c r="W85" s="177">
         <v>40497</v>
@@ -10713,7 +10713,7 @@
       <c r="AM85" s="54"/>
       <c r="AN85" s="54"/>
       <c r="AO85" s="75" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="86" spans="2:41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Anynines (CF v2), Gen override Fix
Fix: Other runtimes could get duplicated
</commit_message>
<xml_diff>
--- a/Cloud Platforms (PaaS).xlsx
+++ b/Cloud Platforms (PaaS).xlsx
@@ -1253,7 +1253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="540">
   <si>
     <t>Parent Platform Name</t>
   </si>
@@ -4222,10 +4222,10 @@
   <dimension ref="A1:AO320"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="S19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="Z16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="AJ18" sqref="AJ18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4539,11 +4539,11 @@
       </c>
       <c r="AH3" s="22">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AI3" s="10">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AJ3" s="23">
         <f t="shared" si="1"/>
@@ -5744,8 +5744,12 @@
       </c>
       <c r="AF18" s="124"/>
       <c r="AG18" s="129"/>
-      <c r="AH18" s="126"/>
-      <c r="AI18" s="124"/>
+      <c r="AH18" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI18" s="124" t="s">
+        <v>25</v>
+      </c>
       <c r="AJ18" s="129"/>
       <c r="AK18" s="126" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Updated Orchestra, Prettify JSON
MOD: Orchestra EOL
</commit_message>
<xml_diff>
--- a/Cloud Platforms (PaaS).xlsx
+++ b/Cloud Platforms (PaaS).xlsx
@@ -4222,10 +4222,10 @@
   <dimension ref="A1:AO320"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="Z16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AJ18" sqref="AJ18"/>
+      <selection pane="bottomRight" activeCell="Q66" sqref="Q66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7980,7 +7980,7 @@
       </c>
       <c r="Z47" s="194">
         <f t="shared" ca="1" si="3"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AA47" s="116" t="s">
         <v>307</v>
@@ -9354,7 +9354,7 @@
       <c r="O66" s="89"/>
       <c r="P66" s="102"/>
       <c r="Q66" s="33" t="s">
-        <v>29</v>
+        <v>215</v>
       </c>
       <c r="R66" s="32" t="s">
         <v>134</v>

</xml_diff>